<commit_message>
Minor changes for bowl game.
</commit_message>
<xml_diff>
--- a/atq_charting_template.xlsx
+++ b/atq_charting_template.xlsx
@@ -103,7 +103,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -130,10 +130,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -198,12 +194,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="2.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="44" style="1" width="3.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="3.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="4.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="4.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="12.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="155.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="51" style="1" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="1" width="4.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="4.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="4.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -223,7 +219,7 @@
       <c r="J1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N1" s="7" t="str">
+      <c r="N1" s="2" t="str">
         <f aca="false">IF(G1="?",_xlfn.CONCAT(AQ1,"Q ",AR1,":",TEXT(AS1,"00")),"")</f>
         <v/>
       </c>
@@ -243,7 +239,7 @@
         <f aca="false">IF(AT1="","",IF(AT2="",AV1,AT1-AT2))</f>
         <v/>
       </c>
-      <c r="BF1" s="8" t="n">
+      <c r="BF1" s="7" t="n">
         <f aca="false">BE1=AV1</f>
         <v>1</v>
       </c>
@@ -267,7 +263,7 @@
         <f aca="false">IF(E2="","",IF(E1="",1,1+J1))</f>
         <v/>
       </c>
-      <c r="N2" s="7" t="str">
+      <c r="N2" s="2" t="str">
         <f aca="false">IF(G2="?",_xlfn.CONCAT(AQ2,"Q ",AR2,":",TEXT(AS2,"00")),"")</f>
         <v/>
       </c>
@@ -287,7 +283,7 @@
         <f aca="false">IF(AT2="","",IF(AT3="",AV2,AT2-AT3))</f>
         <v/>
       </c>
-      <c r="BF2" s="8" t="n">
+      <c r="BF2" s="7" t="n">
         <f aca="false">BE2=AV2</f>
         <v>1</v>
       </c>
@@ -312,7 +308,7 @@
         <f aca="false">IF(E3="","",IF(E2="",1,1+J2))</f>
         <v/>
       </c>
-      <c r="N3" s="7" t="str">
+      <c r="N3" s="2" t="str">
         <f aca="false">IF(G3="?",_xlfn.CONCAT(AQ3,"Q ",AR3,":",TEXT(AS3,"00")),"")</f>
         <v/>
       </c>
@@ -332,7 +328,7 @@
         <f aca="false">IF(AT3="","",IF(AT4="",AV3,AT3-AT4))</f>
         <v/>
       </c>
-      <c r="BF3" s="8" t="n">
+      <c r="BF3" s="7" t="n">
         <f aca="false">BE3=AV3</f>
         <v>1</v>
       </c>
@@ -357,7 +353,7 @@
         <f aca="false">IF(E4="","",IF(E3="",1,1+J3))</f>
         <v/>
       </c>
-      <c r="N4" s="7" t="str">
+      <c r="N4" s="2" t="str">
         <f aca="false">IF(G4="?",_xlfn.CONCAT(AQ4,"Q ",AR4,":",TEXT(AS4,"00")),"")</f>
         <v/>
       </c>
@@ -377,7 +373,7 @@
         <f aca="false">IF(AT4="","",IF(AT5="",AV4,AT4-AT5))</f>
         <v/>
       </c>
-      <c r="BF4" s="8" t="n">
+      <c r="BF4" s="7" t="n">
         <f aca="false">BE4=AV4</f>
         <v>1</v>
       </c>
@@ -402,7 +398,7 @@
         <f aca="false">IF(E5="","",IF(E4="",1,1+J4))</f>
         <v/>
       </c>
-      <c r="N5" s="7" t="str">
+      <c r="N5" s="2" t="str">
         <f aca="false">IF(G5="?",_xlfn.CONCAT(AQ5,"Q ",AR5,":",TEXT(AS5,"00")),"")</f>
         <v/>
       </c>
@@ -422,7 +418,7 @@
         <f aca="false">IF(AT5="","",IF(AT6="",AV5,AT5-AT6))</f>
         <v/>
       </c>
-      <c r="BF5" s="8" t="n">
+      <c r="BF5" s="7" t="n">
         <f aca="false">BE5=AV5</f>
         <v>1</v>
       </c>
@@ -447,7 +443,7 @@
         <f aca="false">IF(E6="","",IF(E5="",1,1+J5))</f>
         <v/>
       </c>
-      <c r="N6" s="7" t="str">
+      <c r="N6" s="2" t="str">
         <f aca="false">IF(G6="?",_xlfn.CONCAT(AQ6,"Q ",AR6,":",TEXT(AS6,"00")),"")</f>
         <v/>
       </c>
@@ -467,7 +463,7 @@
         <f aca="false">IF(AT6="","",IF(AT7="",AV6,AT6-AT7))</f>
         <v/>
       </c>
-      <c r="BF6" s="8" t="n">
+      <c r="BF6" s="7" t="n">
         <f aca="false">BE6=AV6</f>
         <v>1</v>
       </c>
@@ -492,7 +488,7 @@
         <f aca="false">IF(E7="","",IF(E6="",1,1+J6))</f>
         <v/>
       </c>
-      <c r="N7" s="7" t="str">
+      <c r="N7" s="2" t="str">
         <f aca="false">IF(G7="?",_xlfn.CONCAT(AQ7,"Q ",AR7,":",TEXT(AS7,"00")),"")</f>
         <v/>
       </c>
@@ -512,7 +508,7 @@
         <f aca="false">IF(AT7="","",IF(AT8="",AV7,AT7-AT8))</f>
         <v/>
       </c>
-      <c r="BF7" s="8" t="n">
+      <c r="BF7" s="7" t="n">
         <f aca="false">BE7=AV7</f>
         <v>1</v>
       </c>
@@ -537,7 +533,7 @@
         <f aca="false">IF(E8="","",IF(E7="",1,1+J7))</f>
         <v/>
       </c>
-      <c r="N8" s="7" t="str">
+      <c r="N8" s="2" t="str">
         <f aca="false">IF(G8="?",_xlfn.CONCAT(AQ8,"Q ",AR8,":",TEXT(AS8,"00")),"")</f>
         <v/>
       </c>
@@ -557,7 +553,7 @@
         <f aca="false">IF(AT8="","",IF(AT9="",AV8,AT8-AT9))</f>
         <v/>
       </c>
-      <c r="BF8" s="8" t="n">
+      <c r="BF8" s="7" t="n">
         <f aca="false">BE8=AV8</f>
         <v>1</v>
       </c>
@@ -582,7 +578,7 @@
         <f aca="false">IF(E9="","",IF(E8="",1,1+J8))</f>
         <v/>
       </c>
-      <c r="N9" s="7" t="str">
+      <c r="N9" s="2" t="str">
         <f aca="false">IF(G9="?",_xlfn.CONCAT(AQ9,"Q ",AR9,":",TEXT(AS9,"00")),"")</f>
         <v/>
       </c>
@@ -602,7 +598,7 @@
         <f aca="false">IF(AT9="","",IF(AT10="",AV9,AT9-AT10))</f>
         <v/>
       </c>
-      <c r="BF9" s="8" t="n">
+      <c r="BF9" s="7" t="n">
         <f aca="false">BE9=AV9</f>
         <v>1</v>
       </c>
@@ -627,7 +623,7 @@
         <f aca="false">IF(E10="","",IF(E9="",1,1+J9))</f>
         <v/>
       </c>
-      <c r="N10" s="7" t="str">
+      <c r="N10" s="2" t="str">
         <f aca="false">IF(G10="?",_xlfn.CONCAT(AQ10,"Q ",AR10,":",TEXT(AS10,"00")),"")</f>
         <v/>
       </c>
@@ -647,7 +643,7 @@
         <f aca="false">IF(AT10="","",IF(AT11="",AV10,AT10-AT11))</f>
         <v/>
       </c>
-      <c r="BF10" s="8" t="n">
+      <c r="BF10" s="7" t="n">
         <f aca="false">BE10=AV10</f>
         <v>1</v>
       </c>
@@ -672,7 +668,7 @@
         <f aca="false">IF(E11="","",IF(E10="",1,1+J10))</f>
         <v/>
       </c>
-      <c r="N11" s="7" t="str">
+      <c r="N11" s="2" t="str">
         <f aca="false">IF(G11="?",_xlfn.CONCAT(AQ11,"Q ",AR11,":",TEXT(AS11,"00")),"")</f>
         <v/>
       </c>
@@ -692,7 +688,7 @@
         <f aca="false">IF(AT11="","",IF(AT12="",AV11,AT11-AT12))</f>
         <v/>
       </c>
-      <c r="BF11" s="8" t="n">
+      <c r="BF11" s="7" t="n">
         <f aca="false">BE11=AV11</f>
         <v>1</v>
       </c>
@@ -717,7 +713,7 @@
         <f aca="false">IF(E12="","",IF(E11="",1,1+J11))</f>
         <v/>
       </c>
-      <c r="N12" s="7" t="str">
+      <c r="N12" s="2" t="str">
         <f aca="false">IF(G12="?",_xlfn.CONCAT(AQ12,"Q ",AR12,":",TEXT(AS12,"00")),"")</f>
         <v/>
       </c>
@@ -737,7 +733,7 @@
         <f aca="false">IF(AT12="","",IF(AT13="",AV12,AT12-AT13))</f>
         <v/>
       </c>
-      <c r="BF12" s="8" t="n">
+      <c r="BF12" s="7" t="n">
         <f aca="false">BE12=AV12</f>
         <v>1</v>
       </c>
@@ -762,7 +758,7 @@
         <f aca="false">IF(E13="","",IF(E12="",1,1+J12))</f>
         <v/>
       </c>
-      <c r="N13" s="7" t="str">
+      <c r="N13" s="2" t="str">
         <f aca="false">IF(G13="?",_xlfn.CONCAT(AQ13,"Q ",AR13,":",TEXT(AS13,"00")),"")</f>
         <v/>
       </c>
@@ -782,7 +778,7 @@
         <f aca="false">IF(AT13="","",IF(AT14="",AV13,AT13-AT14))</f>
         <v/>
       </c>
-      <c r="BF13" s="8" t="n">
+      <c r="BF13" s="7" t="n">
         <f aca="false">BE13=AV13</f>
         <v>1</v>
       </c>
@@ -807,7 +803,7 @@
         <f aca="false">IF(E14="","",IF(E13="",1,1+J13))</f>
         <v/>
       </c>
-      <c r="N14" s="7" t="str">
+      <c r="N14" s="2" t="str">
         <f aca="false">IF(G14="?",_xlfn.CONCAT(AQ14,"Q ",AR14,":",TEXT(AS14,"00")),"")</f>
         <v/>
       </c>
@@ -827,7 +823,7 @@
         <f aca="false">IF(AT14="","",IF(AT15="",AV14,AT14-AT15))</f>
         <v/>
       </c>
-      <c r="BF14" s="8" t="n">
+      <c r="BF14" s="7" t="n">
         <f aca="false">BE14=AV14</f>
         <v>1</v>
       </c>
@@ -852,7 +848,7 @@
         <f aca="false">IF(E15="","",IF(E14="",1,1+J14))</f>
         <v/>
       </c>
-      <c r="N15" s="7" t="str">
+      <c r="N15" s="2" t="str">
         <f aca="false">IF(G15="?",_xlfn.CONCAT(AQ15,"Q ",AR15,":",TEXT(AS15,"00")),"")</f>
         <v/>
       </c>
@@ -872,7 +868,7 @@
         <f aca="false">IF(AT15="","",IF(AT16="",AV15,AT15-AT16))</f>
         <v/>
       </c>
-      <c r="BF15" s="8" t="n">
+      <c r="BF15" s="7" t="n">
         <f aca="false">BE15=AV15</f>
         <v>1</v>
       </c>
@@ -897,7 +893,7 @@
         <f aca="false">IF(E16="","",IF(E15="",1,1+J15))</f>
         <v/>
       </c>
-      <c r="N16" s="7" t="str">
+      <c r="N16" s="2" t="str">
         <f aca="false">IF(G16="?",_xlfn.CONCAT(AQ16,"Q ",AR16,":",TEXT(AS16,"00")),"")</f>
         <v/>
       </c>
@@ -917,7 +913,7 @@
         <f aca="false">IF(AT16="","",IF(AT17="",AV16,AT16-AT17))</f>
         <v/>
       </c>
-      <c r="BF16" s="8" t="n">
+      <c r="BF16" s="7" t="n">
         <f aca="false">BE16=AV16</f>
         <v>1</v>
       </c>
@@ -942,7 +938,7 @@
         <f aca="false">IF(E17="","",IF(E16="",1,1+J16))</f>
         <v/>
       </c>
-      <c r="N17" s="7" t="str">
+      <c r="N17" s="2" t="str">
         <f aca="false">IF(G17="?",_xlfn.CONCAT(AQ17,"Q ",AR17,":",TEXT(AS17,"00")),"")</f>
         <v/>
       </c>
@@ -962,7 +958,7 @@
         <f aca="false">IF(AT17="","",IF(AT18="",AV17,AT17-AT18))</f>
         <v/>
       </c>
-      <c r="BF17" s="8" t="n">
+      <c r="BF17" s="7" t="n">
         <f aca="false">BE17=AV17</f>
         <v>1</v>
       </c>
@@ -987,7 +983,7 @@
         <f aca="false">IF(E18="","",IF(E17="",1,1+J17))</f>
         <v/>
       </c>
-      <c r="N18" s="7" t="str">
+      <c r="N18" s="2" t="str">
         <f aca="false">IF(G18="?",_xlfn.CONCAT(AQ18,"Q ",AR18,":",TEXT(AS18,"00")),"")</f>
         <v/>
       </c>
@@ -1007,7 +1003,7 @@
         <f aca="false">IF(AT18="","",IF(AT19="",AV18,AT18-AT19))</f>
         <v/>
       </c>
-      <c r="BF18" s="8" t="n">
+      <c r="BF18" s="7" t="n">
         <f aca="false">BE18=AV18</f>
         <v>1</v>
       </c>
@@ -1032,7 +1028,7 @@
         <f aca="false">IF(E19="","",IF(E18="",1,1+J18))</f>
         <v/>
       </c>
-      <c r="N19" s="7" t="str">
+      <c r="N19" s="2" t="str">
         <f aca="false">IF(G19="?",_xlfn.CONCAT(AQ19,"Q ",AR19,":",TEXT(AS19,"00")),"")</f>
         <v/>
       </c>
@@ -1052,7 +1048,7 @@
         <f aca="false">IF(AT19="","",IF(AT20="",AV19,AT19-AT20))</f>
         <v/>
       </c>
-      <c r="BF19" s="8" t="n">
+      <c r="BF19" s="7" t="n">
         <f aca="false">BE19=AV19</f>
         <v>1</v>
       </c>
@@ -1077,7 +1073,7 @@
         <f aca="false">IF(E20="","",IF(E19="",1,1+J19))</f>
         <v/>
       </c>
-      <c r="N20" s="7" t="str">
+      <c r="N20" s="2" t="str">
         <f aca="false">IF(G20="?",_xlfn.CONCAT(AQ20,"Q ",AR20,":",TEXT(AS20,"00")),"")</f>
         <v/>
       </c>
@@ -1097,7 +1093,7 @@
         <f aca="false">IF(AT20="","",IF(AT21="",AV20,AT20-AT21))</f>
         <v/>
       </c>
-      <c r="BF20" s="8" t="n">
+      <c r="BF20" s="7" t="n">
         <f aca="false">BE20=AV20</f>
         <v>1</v>
       </c>
@@ -1122,7 +1118,7 @@
         <f aca="false">IF(E21="","",IF(E20="",1,1+J20))</f>
         <v/>
       </c>
-      <c r="N21" s="7" t="str">
+      <c r="N21" s="2" t="str">
         <f aca="false">IF(G21="?",_xlfn.CONCAT(AQ21,"Q ",AR21,":",TEXT(AS21,"00")),"")</f>
         <v/>
       </c>
@@ -1142,7 +1138,7 @@
         <f aca="false">IF(AT21="","",IF(AT22="",AV21,AT21-AT22))</f>
         <v/>
       </c>
-      <c r="BF21" s="8" t="n">
+      <c r="BF21" s="7" t="n">
         <f aca="false">BE21=AV21</f>
         <v>1</v>
       </c>
@@ -1167,7 +1163,7 @@
         <f aca="false">IF(E22="","",IF(E21="",1,1+J21))</f>
         <v/>
       </c>
-      <c r="N22" s="7" t="str">
+      <c r="N22" s="2" t="str">
         <f aca="false">IF(G22="?",_xlfn.CONCAT(AQ22,"Q ",AR22,":",TEXT(AS22,"00")),"")</f>
         <v/>
       </c>
@@ -1187,7 +1183,7 @@
         <f aca="false">IF(AT22="","",IF(AT23="",AV22,AT22-AT23))</f>
         <v/>
       </c>
-      <c r="BF22" s="8" t="n">
+      <c r="BF22" s="7" t="n">
         <f aca="false">BE22=AV22</f>
         <v>1</v>
       </c>
@@ -1212,7 +1208,7 @@
         <f aca="false">IF(E23="","",IF(E22="",1,1+J22))</f>
         <v/>
       </c>
-      <c r="N23" s="7" t="str">
+      <c r="N23" s="2" t="str">
         <f aca="false">IF(G23="?",_xlfn.CONCAT(AQ23,"Q ",AR23,":",TEXT(AS23,"00")),"")</f>
         <v/>
       </c>
@@ -1232,7 +1228,7 @@
         <f aca="false">IF(AT23="","",IF(AT24="",AV23,AT23-AT24))</f>
         <v/>
       </c>
-      <c r="BF23" s="8" t="n">
+      <c r="BF23" s="7" t="n">
         <f aca="false">BE23=AV23</f>
         <v>1</v>
       </c>
@@ -1257,7 +1253,7 @@
         <f aca="false">IF(E24="","",IF(E23="",1,1+J23))</f>
         <v/>
       </c>
-      <c r="N24" s="7" t="str">
+      <c r="N24" s="2" t="str">
         <f aca="false">IF(G24="?",_xlfn.CONCAT(AQ24,"Q ",AR24,":",TEXT(AS24,"00")),"")</f>
         <v/>
       </c>
@@ -1277,7 +1273,7 @@
         <f aca="false">IF(AT24="","",IF(AT25="",AV24,AT24-AT25))</f>
         <v/>
       </c>
-      <c r="BF24" s="8" t="n">
+      <c r="BF24" s="7" t="n">
         <f aca="false">BE24=AV24</f>
         <v>1</v>
       </c>
@@ -1302,7 +1298,7 @@
         <f aca="false">IF(E25="","",IF(E24="",1,1+J24))</f>
         <v/>
       </c>
-      <c r="N25" s="7" t="str">
+      <c r="N25" s="2" t="str">
         <f aca="false">IF(G25="?",_xlfn.CONCAT(AQ25,"Q ",AR25,":",TEXT(AS25,"00")),"")</f>
         <v/>
       </c>
@@ -1322,7 +1318,7 @@
         <f aca="false">IF(AT25="","",IF(AT26="",AV25,AT25-AT26))</f>
         <v/>
       </c>
-      <c r="BF25" s="8" t="n">
+      <c r="BF25" s="7" t="n">
         <f aca="false">BE25=AV25</f>
         <v>1</v>
       </c>
@@ -1347,7 +1343,7 @@
         <f aca="false">IF(E26="","",IF(E25="",1,1+J25))</f>
         <v/>
       </c>
-      <c r="N26" s="7" t="str">
+      <c r="N26" s="2" t="str">
         <f aca="false">IF(G26="?",_xlfn.CONCAT(AQ26,"Q ",AR26,":",TEXT(AS26,"00")),"")</f>
         <v/>
       </c>
@@ -1367,7 +1363,7 @@
         <f aca="false">IF(AT26="","",IF(AT27="",AV26,AT26-AT27))</f>
         <v/>
       </c>
-      <c r="BF26" s="8" t="n">
+      <c r="BF26" s="7" t="n">
         <f aca="false">BE26=AV26</f>
         <v>1</v>
       </c>
@@ -1392,7 +1388,7 @@
         <f aca="false">IF(E27="","",IF(E26="",1,1+J26))</f>
         <v/>
       </c>
-      <c r="N27" s="7" t="str">
+      <c r="N27" s="2" t="str">
         <f aca="false">IF(G27="?",_xlfn.CONCAT(AQ27,"Q ",AR27,":",TEXT(AS27,"00")),"")</f>
         <v/>
       </c>
@@ -1412,7 +1408,7 @@
         <f aca="false">IF(AT27="","",IF(AT28="",AV27,AT27-AT28))</f>
         <v/>
       </c>
-      <c r="BF27" s="8" t="n">
+      <c r="BF27" s="7" t="n">
         <f aca="false">BE27=AV27</f>
         <v>1</v>
       </c>
@@ -1437,7 +1433,7 @@
         <f aca="false">IF(E28="","",IF(E27="",1,1+J27))</f>
         <v/>
       </c>
-      <c r="N28" s="7" t="str">
+      <c r="N28" s="2" t="str">
         <f aca="false">IF(G28="?",_xlfn.CONCAT(AQ28,"Q ",AR28,":",TEXT(AS28,"00")),"")</f>
         <v/>
       </c>
@@ -1457,7 +1453,7 @@
         <f aca="false">IF(AT28="","",IF(AT29="",AV28,AT28-AT29))</f>
         <v/>
       </c>
-      <c r="BF28" s="8" t="n">
+      <c r="BF28" s="7" t="n">
         <f aca="false">BE28=AV28</f>
         <v>1</v>
       </c>
@@ -1482,7 +1478,7 @@
         <f aca="false">IF(E29="","",IF(E28="",1,1+J28))</f>
         <v/>
       </c>
-      <c r="N29" s="7" t="str">
+      <c r="N29" s="2" t="str">
         <f aca="false">IF(G29="?",_xlfn.CONCAT(AQ29,"Q ",AR29,":",TEXT(AS29,"00")),"")</f>
         <v/>
       </c>
@@ -1502,7 +1498,7 @@
         <f aca="false">IF(AT29="","",IF(AT30="",AV29,AT29-AT30))</f>
         <v/>
       </c>
-      <c r="BF29" s="8" t="n">
+      <c r="BF29" s="7" t="n">
         <f aca="false">BE29=AV29</f>
         <v>1</v>
       </c>
@@ -1527,7 +1523,7 @@
         <f aca="false">IF(E30="","",IF(E29="",1,1+J29))</f>
         <v/>
       </c>
-      <c r="N30" s="7" t="str">
+      <c r="N30" s="2" t="str">
         <f aca="false">IF(G30="?",_xlfn.CONCAT(AQ30,"Q ",AR30,":",TEXT(AS30,"00")),"")</f>
         <v/>
       </c>
@@ -1547,7 +1543,7 @@
         <f aca="false">IF(AT30="","",IF(AT31="",AV30,AT30-AT31))</f>
         <v/>
       </c>
-      <c r="BF30" s="8" t="n">
+      <c r="BF30" s="7" t="n">
         <f aca="false">BE30=AV30</f>
         <v>1</v>
       </c>
@@ -1572,7 +1568,7 @@
         <f aca="false">IF(E31="","",IF(E30="",1,1+J30))</f>
         <v/>
       </c>
-      <c r="N31" s="7" t="str">
+      <c r="N31" s="2" t="str">
         <f aca="false">IF(G31="?",_xlfn.CONCAT(AQ31,"Q ",AR31,":",TEXT(AS31,"00")),"")</f>
         <v/>
       </c>
@@ -1592,7 +1588,7 @@
         <f aca="false">IF(AT31="","",IF(AT32="",AV31,AT31-AT32))</f>
         <v/>
       </c>
-      <c r="BF31" s="8" t="n">
+      <c r="BF31" s="7" t="n">
         <f aca="false">BE31=AV31</f>
         <v>1</v>
       </c>
@@ -1617,7 +1613,7 @@
         <f aca="false">IF(E32="","",IF(E31="",1,1+J31))</f>
         <v/>
       </c>
-      <c r="N32" s="7" t="str">
+      <c r="N32" s="2" t="str">
         <f aca="false">IF(G32="?",_xlfn.CONCAT(AQ32,"Q ",AR32,":",TEXT(AS32,"00")),"")</f>
         <v/>
       </c>
@@ -1637,7 +1633,7 @@
         <f aca="false">IF(AT32="","",IF(AT33="",AV32,AT32-AT33))</f>
         <v/>
       </c>
-      <c r="BF32" s="8" t="n">
+      <c r="BF32" s="7" t="n">
         <f aca="false">BE32=AV32</f>
         <v>1</v>
       </c>
@@ -1662,7 +1658,7 @@
         <f aca="false">IF(E33="","",IF(E32="",1,1+J32))</f>
         <v/>
       </c>
-      <c r="N33" s="7" t="str">
+      <c r="N33" s="2" t="str">
         <f aca="false">IF(G33="?",_xlfn.CONCAT(AQ33,"Q ",AR33,":",TEXT(AS33,"00")),"")</f>
         <v/>
       </c>
@@ -1682,7 +1678,7 @@
         <f aca="false">IF(AT33="","",IF(AT34="",AV33,AT33-AT34))</f>
         <v/>
       </c>
-      <c r="BF33" s="8" t="n">
+      <c r="BF33" s="7" t="n">
         <f aca="false">BE33=AV33</f>
         <v>1</v>
       </c>
@@ -1707,7 +1703,7 @@
         <f aca="false">IF(E34="","",IF(E33="",1,1+J33))</f>
         <v/>
       </c>
-      <c r="N34" s="7" t="str">
+      <c r="N34" s="2" t="str">
         <f aca="false">IF(G34="?",_xlfn.CONCAT(AQ34,"Q ",AR34,":",TEXT(AS34,"00")),"")</f>
         <v/>
       </c>
@@ -1727,7 +1723,7 @@
         <f aca="false">IF(AT34="","",IF(AT35="",AV34,AT34-AT35))</f>
         <v/>
       </c>
-      <c r="BF34" s="8" t="n">
+      <c r="BF34" s="7" t="n">
         <f aca="false">BE34=AV34</f>
         <v>1</v>
       </c>
@@ -1752,7 +1748,7 @@
         <f aca="false">IF(E35="","",IF(E34="",1,1+J34))</f>
         <v/>
       </c>
-      <c r="N35" s="7" t="str">
+      <c r="N35" s="2" t="str">
         <f aca="false">IF(G35="?",_xlfn.CONCAT(AQ35,"Q ",AR35,":",TEXT(AS35,"00")),"")</f>
         <v/>
       </c>
@@ -1772,7 +1768,7 @@
         <f aca="false">IF(AT35="","",IF(AT36="",AV35,AT35-AT36))</f>
         <v/>
       </c>
-      <c r="BF35" s="8" t="n">
+      <c r="BF35" s="7" t="n">
         <f aca="false">BE35=AV35</f>
         <v>1</v>
       </c>
@@ -1797,7 +1793,7 @@
         <f aca="false">IF(E36="","",IF(E35="",1,1+J35))</f>
         <v/>
       </c>
-      <c r="N36" s="7" t="str">
+      <c r="N36" s="2" t="str">
         <f aca="false">IF(G36="?",_xlfn.CONCAT(AQ36,"Q ",AR36,":",TEXT(AS36,"00")),"")</f>
         <v/>
       </c>
@@ -1817,7 +1813,7 @@
         <f aca="false">IF(AT36="","",IF(AT37="",AV36,AT36-AT37))</f>
         <v/>
       </c>
-      <c r="BF36" s="8" t="n">
+      <c r="BF36" s="7" t="n">
         <f aca="false">BE36=AV36</f>
         <v>1</v>
       </c>
@@ -1842,7 +1838,7 @@
         <f aca="false">IF(E37="","",IF(E36="",1,1+J36))</f>
         <v/>
       </c>
-      <c r="N37" s="7" t="str">
+      <c r="N37" s="2" t="str">
         <f aca="false">IF(G37="?",_xlfn.CONCAT(AQ37,"Q ",AR37,":",TEXT(AS37,"00")),"")</f>
         <v/>
       </c>
@@ -1862,7 +1858,7 @@
         <f aca="false">IF(AT37="","",IF(AT38="",AV37,AT37-AT38))</f>
         <v/>
       </c>
-      <c r="BF37" s="8" t="n">
+      <c r="BF37" s="7" t="n">
         <f aca="false">BE37=AV37</f>
         <v>1</v>
       </c>
@@ -1887,7 +1883,7 @@
         <f aca="false">IF(E38="","",IF(E37="",1,1+J37))</f>
         <v/>
       </c>
-      <c r="N38" s="7" t="str">
+      <c r="N38" s="2" t="str">
         <f aca="false">IF(G38="?",_xlfn.CONCAT(AQ38,"Q ",AR38,":",TEXT(AS38,"00")),"")</f>
         <v/>
       </c>
@@ -1907,7 +1903,7 @@
         <f aca="false">IF(AT38="","",IF(AT39="",AV38,AT38-AT39))</f>
         <v/>
       </c>
-      <c r="BF38" s="8" t="n">
+      <c r="BF38" s="7" t="n">
         <f aca="false">BE38=AV38</f>
         <v>1</v>
       </c>
@@ -1932,7 +1928,7 @@
         <f aca="false">IF(E39="","",IF(E38="",1,1+J38))</f>
         <v/>
       </c>
-      <c r="N39" s="7" t="str">
+      <c r="N39" s="2" t="str">
         <f aca="false">IF(G39="?",_xlfn.CONCAT(AQ39,"Q ",AR39,":",TEXT(AS39,"00")),"")</f>
         <v/>
       </c>
@@ -1952,7 +1948,7 @@
         <f aca="false">IF(AT39="","",IF(AT40="",AV39,AT39-AT40))</f>
         <v/>
       </c>
-      <c r="BF39" s="8" t="n">
+      <c r="BF39" s="7" t="n">
         <f aca="false">BE39=AV39</f>
         <v>1</v>
       </c>
@@ -1977,7 +1973,7 @@
         <f aca="false">IF(E40="","",IF(E39="",1,1+J39))</f>
         <v/>
       </c>
-      <c r="N40" s="7" t="str">
+      <c r="N40" s="2" t="str">
         <f aca="false">IF(G40="?",_xlfn.CONCAT(AQ40,"Q ",AR40,":",TEXT(AS40,"00")),"")</f>
         <v/>
       </c>
@@ -1997,7 +1993,7 @@
         <f aca="false">IF(AT40="","",IF(AT41="",AV40,AT40-AT41))</f>
         <v/>
       </c>
-      <c r="BF40" s="8" t="n">
+      <c r="BF40" s="7" t="n">
         <f aca="false">BE40=AV40</f>
         <v>1</v>
       </c>
@@ -2022,7 +2018,7 @@
         <f aca="false">IF(E41="","",IF(E40="",1,1+J40))</f>
         <v/>
       </c>
-      <c r="N41" s="7" t="str">
+      <c r="N41" s="2" t="str">
         <f aca="false">IF(G41="?",_xlfn.CONCAT(AQ41,"Q ",AR41,":",TEXT(AS41,"00")),"")</f>
         <v/>
       </c>
@@ -2042,7 +2038,7 @@
         <f aca="false">IF(AT41="","",IF(AT42="",AV41,AT41-AT42))</f>
         <v/>
       </c>
-      <c r="BF41" s="8" t="n">
+      <c r="BF41" s="7" t="n">
         <f aca="false">BE41=AV41</f>
         <v>1</v>
       </c>
@@ -2067,7 +2063,7 @@
         <f aca="false">IF(E42="","",IF(E41="",1,1+J41))</f>
         <v/>
       </c>
-      <c r="N42" s="7" t="str">
+      <c r="N42" s="2" t="str">
         <f aca="false">IF(G42="?",_xlfn.CONCAT(AQ42,"Q ",AR42,":",TEXT(AS42,"00")),"")</f>
         <v/>
       </c>
@@ -2087,7 +2083,7 @@
         <f aca="false">IF(AT42="","",IF(AT43="",AV42,AT42-AT43))</f>
         <v/>
       </c>
-      <c r="BF42" s="8" t="n">
+      <c r="BF42" s="7" t="n">
         <f aca="false">BE42=AV42</f>
         <v>1</v>
       </c>
@@ -2112,7 +2108,7 @@
         <f aca="false">IF(E43="","",IF(E42="",1,1+J42))</f>
         <v/>
       </c>
-      <c r="N43" s="7" t="str">
+      <c r="N43" s="2" t="str">
         <f aca="false">IF(G43="?",_xlfn.CONCAT(AQ43,"Q ",AR43,":",TEXT(AS43,"00")),"")</f>
         <v/>
       </c>
@@ -2132,7 +2128,7 @@
         <f aca="false">IF(AT43="","",IF(AT44="",AV43,AT43-AT44))</f>
         <v/>
       </c>
-      <c r="BF43" s="8" t="n">
+      <c r="BF43" s="7" t="n">
         <f aca="false">BE43=AV43</f>
         <v>1</v>
       </c>
@@ -2157,7 +2153,7 @@
         <f aca="false">IF(E44="","",IF(E43="",1,1+J43))</f>
         <v/>
       </c>
-      <c r="N44" s="7" t="str">
+      <c r="N44" s="2" t="str">
         <f aca="false">IF(G44="?",_xlfn.CONCAT(AQ44,"Q ",AR44,":",TEXT(AS44,"00")),"")</f>
         <v/>
       </c>
@@ -2177,7 +2173,7 @@
         <f aca="false">IF(AT44="","",IF(AT45="",AV44,AT44-AT45))</f>
         <v/>
       </c>
-      <c r="BF44" s="8" t="n">
+      <c r="BF44" s="7" t="n">
         <f aca="false">BE44=AV44</f>
         <v>1</v>
       </c>
@@ -2202,7 +2198,7 @@
         <f aca="false">IF(E45="","",IF(E44="",1,1+J44))</f>
         <v/>
       </c>
-      <c r="N45" s="7" t="str">
+      <c r="N45" s="2" t="str">
         <f aca="false">IF(G45="?",_xlfn.CONCAT(AQ45,"Q ",AR45,":",TEXT(AS45,"00")),"")</f>
         <v/>
       </c>
@@ -2222,7 +2218,7 @@
         <f aca="false">IF(AT45="","",IF(AT46="",AV45,AT45-AT46))</f>
         <v/>
       </c>
-      <c r="BF45" s="8" t="n">
+      <c r="BF45" s="7" t="n">
         <f aca="false">BE45=AV45</f>
         <v>1</v>
       </c>
@@ -2247,7 +2243,7 @@
         <f aca="false">IF(E46="","",IF(E45="",1,1+J45))</f>
         <v/>
       </c>
-      <c r="N46" s="7" t="str">
+      <c r="N46" s="2" t="str">
         <f aca="false">IF(G46="?",_xlfn.CONCAT(AQ46,"Q ",AR46,":",TEXT(AS46,"00")),"")</f>
         <v/>
       </c>
@@ -2267,7 +2263,7 @@
         <f aca="false">IF(AT46="","",IF(AT47="",AV46,AT46-AT47))</f>
         <v/>
       </c>
-      <c r="BF46" s="8" t="n">
+      <c r="BF46" s="7" t="n">
         <f aca="false">BE46=AV46</f>
         <v>1</v>
       </c>
@@ -2292,7 +2288,7 @@
         <f aca="false">IF(E47="","",IF(E46="",1,1+J46))</f>
         <v/>
       </c>
-      <c r="N47" s="7" t="str">
+      <c r="N47" s="2" t="str">
         <f aca="false">IF(G47="?",_xlfn.CONCAT(AQ47,"Q ",AR47,":",TEXT(AS47,"00")),"")</f>
         <v/>
       </c>
@@ -2312,7 +2308,7 @@
         <f aca="false">IF(AT47="","",IF(AT48="",AV47,AT47-AT48))</f>
         <v/>
       </c>
-      <c r="BF47" s="8" t="n">
+      <c r="BF47" s="7" t="n">
         <f aca="false">BE47=AV47</f>
         <v>1</v>
       </c>
@@ -2337,7 +2333,7 @@
         <f aca="false">IF(E48="","",IF(E47="",1,1+J47))</f>
         <v/>
       </c>
-      <c r="N48" s="7" t="str">
+      <c r="N48" s="2" t="str">
         <f aca="false">IF(G48="?",_xlfn.CONCAT(AQ48,"Q ",AR48,":",TEXT(AS48,"00")),"")</f>
         <v/>
       </c>
@@ -2357,7 +2353,7 @@
         <f aca="false">IF(AT48="","",IF(AT49="",AV48,AT48-AT49))</f>
         <v/>
       </c>
-      <c r="BF48" s="8" t="n">
+      <c r="BF48" s="7" t="n">
         <f aca="false">BE48=AV48</f>
         <v>1</v>
       </c>
@@ -2382,7 +2378,7 @@
         <f aca="false">IF(E49="","",IF(E48="",1,1+J48))</f>
         <v/>
       </c>
-      <c r="N49" s="7" t="str">
+      <c r="N49" s="2" t="str">
         <f aca="false">IF(G49="?",_xlfn.CONCAT(AQ49,"Q ",AR49,":",TEXT(AS49,"00")),"")</f>
         <v/>
       </c>
@@ -2402,7 +2398,7 @@
         <f aca="false">IF(AT49="","",IF(AT50="",AV49,AT49-AT50))</f>
         <v/>
       </c>
-      <c r="BF49" s="8" t="n">
+      <c r="BF49" s="7" t="n">
         <f aca="false">BE49=AV49</f>
         <v>1</v>
       </c>
@@ -2427,7 +2423,7 @@
         <f aca="false">IF(E50="","",IF(E49="",1,1+J49))</f>
         <v/>
       </c>
-      <c r="N50" s="7" t="str">
+      <c r="N50" s="2" t="str">
         <f aca="false">IF(G50="?",_xlfn.CONCAT(AQ50,"Q ",AR50,":",TEXT(AS50,"00")),"")</f>
         <v/>
       </c>
@@ -2447,7 +2443,7 @@
         <f aca="false">IF(AT50="","",IF(AT51="",AV50,AT50-AT51))</f>
         <v/>
       </c>
-      <c r="BF50" s="8" t="n">
+      <c r="BF50" s="7" t="n">
         <f aca="false">BE50=AV50</f>
         <v>1</v>
       </c>
@@ -2472,7 +2468,7 @@
         <f aca="false">IF(E51="","",IF(E50="",1,1+J50))</f>
         <v/>
       </c>
-      <c r="N51" s="7" t="str">
+      <c r="N51" s="2" t="str">
         <f aca="false">IF(G51="?",_xlfn.CONCAT(AQ51,"Q ",AR51,":",TEXT(AS51,"00")),"")</f>
         <v/>
       </c>
@@ -2492,7 +2488,7 @@
         <f aca="false">IF(AT51="","",IF(AT52="",AV51,AT51-AT52))</f>
         <v/>
       </c>
-      <c r="BF51" s="8" t="n">
+      <c r="BF51" s="7" t="n">
         <f aca="false">BE51=AV51</f>
         <v>1</v>
       </c>
@@ -2517,7 +2513,7 @@
         <f aca="false">IF(E52="","",IF(E51="",1,1+J51))</f>
         <v/>
       </c>
-      <c r="N52" s="7" t="str">
+      <c r="N52" s="2" t="str">
         <f aca="false">IF(G52="?",_xlfn.CONCAT(AQ52,"Q ",AR52,":",TEXT(AS52,"00")),"")</f>
         <v/>
       </c>
@@ -2537,7 +2533,7 @@
         <f aca="false">IF(AT52="","",IF(AT53="",AV52,AT52-AT53))</f>
         <v/>
       </c>
-      <c r="BF52" s="8" t="n">
+      <c r="BF52" s="7" t="n">
         <f aca="false">BE52=AV52</f>
         <v>1</v>
       </c>
@@ -2562,7 +2558,7 @@
         <f aca="false">IF(E53="","",IF(E52="",1,1+J52))</f>
         <v/>
       </c>
-      <c r="N53" s="7" t="str">
+      <c r="N53" s="2" t="str">
         <f aca="false">IF(G53="?",_xlfn.CONCAT(AQ53,"Q ",AR53,":",TEXT(AS53,"00")),"")</f>
         <v/>
       </c>
@@ -2582,7 +2578,7 @@
         <f aca="false">IF(AT53="","",IF(AT54="",AV53,AT53-AT54))</f>
         <v/>
       </c>
-      <c r="BF53" s="8" t="n">
+      <c r="BF53" s="7" t="n">
         <f aca="false">BE53=AV53</f>
         <v>1</v>
       </c>
@@ -2607,7 +2603,7 @@
         <f aca="false">IF(E54="","",IF(E53="",1,1+J53))</f>
         <v/>
       </c>
-      <c r="N54" s="7" t="str">
+      <c r="N54" s="2" t="str">
         <f aca="false">IF(G54="?",_xlfn.CONCAT(AQ54,"Q ",AR54,":",TEXT(AS54,"00")),"")</f>
         <v/>
       </c>
@@ -2627,7 +2623,7 @@
         <f aca="false">IF(AT54="","",IF(AT55="",AV54,AT54-AT55))</f>
         <v/>
       </c>
-      <c r="BF54" s="8" t="n">
+      <c r="BF54" s="7" t="n">
         <f aca="false">BE54=AV54</f>
         <v>1</v>
       </c>
@@ -2652,7 +2648,7 @@
         <f aca="false">IF(E55="","",IF(E54="",1,1+J54))</f>
         <v/>
       </c>
-      <c r="N55" s="7" t="str">
+      <c r="N55" s="2" t="str">
         <f aca="false">IF(G55="?",_xlfn.CONCAT(AQ55,"Q ",AR55,":",TEXT(AS55,"00")),"")</f>
         <v/>
       </c>
@@ -2672,7 +2668,7 @@
         <f aca="false">IF(AT55="","",IF(AT56="",AV55,AT55-AT56))</f>
         <v/>
       </c>
-      <c r="BF55" s="8" t="n">
+      <c r="BF55" s="7" t="n">
         <f aca="false">BE55=AV55</f>
         <v>1</v>
       </c>
@@ -2697,7 +2693,7 @@
         <f aca="false">IF(E56="","",IF(E55="",1,1+J55))</f>
         <v/>
       </c>
-      <c r="N56" s="7" t="str">
+      <c r="N56" s="2" t="str">
         <f aca="false">IF(G56="?",_xlfn.CONCAT(AQ56,"Q ",AR56,":",TEXT(AS56,"00")),"")</f>
         <v/>
       </c>
@@ -2717,7 +2713,7 @@
         <f aca="false">IF(AT56="","",IF(AT57="",AV56,AT56-AT57))</f>
         <v/>
       </c>
-      <c r="BF56" s="8" t="n">
+      <c r="BF56" s="7" t="n">
         <f aca="false">BE56=AV56</f>
         <v>1</v>
       </c>
@@ -2742,7 +2738,7 @@
         <f aca="false">IF(E57="","",IF(E56="",1,1+J56))</f>
         <v/>
       </c>
-      <c r="N57" s="7" t="str">
+      <c r="N57" s="2" t="str">
         <f aca="false">IF(G57="?",_xlfn.CONCAT(AQ57,"Q ",AR57,":",TEXT(AS57,"00")),"")</f>
         <v/>
       </c>
@@ -2762,7 +2758,7 @@
         <f aca="false">IF(AT57="","",IF(AT58="",AV57,AT57-AT58))</f>
         <v/>
       </c>
-      <c r="BF57" s="8" t="n">
+      <c r="BF57" s="7" t="n">
         <f aca="false">BE57=AV57</f>
         <v>1</v>
       </c>
@@ -2787,7 +2783,7 @@
         <f aca="false">IF(E58="","",IF(E57="",1,1+J57))</f>
         <v/>
       </c>
-      <c r="N58" s="7" t="str">
+      <c r="N58" s="2" t="str">
         <f aca="false">IF(G58="?",_xlfn.CONCAT(AQ58,"Q ",AR58,":",TEXT(AS58,"00")),"")</f>
         <v/>
       </c>
@@ -2807,7 +2803,7 @@
         <f aca="false">IF(AT58="","",IF(AT59="",AV58,AT58-AT59))</f>
         <v/>
       </c>
-      <c r="BF58" s="8" t="n">
+      <c r="BF58" s="7" t="n">
         <f aca="false">BE58=AV58</f>
         <v>1</v>
       </c>
@@ -2832,7 +2828,7 @@
         <f aca="false">IF(E59="","",IF(E58="",1,1+J58))</f>
         <v/>
       </c>
-      <c r="N59" s="7" t="str">
+      <c r="N59" s="2" t="str">
         <f aca="false">IF(G59="?",_xlfn.CONCAT(AQ59,"Q ",AR59,":",TEXT(AS59,"00")),"")</f>
         <v/>
       </c>
@@ -2852,7 +2848,7 @@
         <f aca="false">IF(AT59="","",IF(AT60="",AV59,AT59-AT60))</f>
         <v/>
       </c>
-      <c r="BF59" s="8" t="n">
+      <c r="BF59" s="7" t="n">
         <f aca="false">BE59=AV59</f>
         <v>1</v>
       </c>
@@ -2877,7 +2873,7 @@
         <f aca="false">IF(E60="","",IF(E59="",1,1+J59))</f>
         <v/>
       </c>
-      <c r="N60" s="7" t="str">
+      <c r="N60" s="2" t="str">
         <f aca="false">IF(G60="?",_xlfn.CONCAT(AQ60,"Q ",AR60,":",TEXT(AS60,"00")),"")</f>
         <v/>
       </c>
@@ -2897,7 +2893,7 @@
         <f aca="false">IF(AT60="","",IF(AT61="",AV60,AT60-AT61))</f>
         <v/>
       </c>
-      <c r="BF60" s="8" t="n">
+      <c r="BF60" s="7" t="n">
         <f aca="false">BE60=AV60</f>
         <v>1</v>
       </c>
@@ -2922,7 +2918,7 @@
         <f aca="false">IF(E61="","",IF(E60="",1,1+J60))</f>
         <v/>
       </c>
-      <c r="N61" s="7" t="str">
+      <c r="N61" s="2" t="str">
         <f aca="false">IF(G61="?",_xlfn.CONCAT(AQ61,"Q ",AR61,":",TEXT(AS61,"00")),"")</f>
         <v/>
       </c>
@@ -2942,7 +2938,7 @@
         <f aca="false">IF(AT61="","",IF(AT62="",AV61,AT61-AT62))</f>
         <v/>
       </c>
-      <c r="BF61" s="8" t="n">
+      <c r="BF61" s="7" t="n">
         <f aca="false">BE61=AV61</f>
         <v>1</v>
       </c>
@@ -2967,7 +2963,7 @@
         <f aca="false">IF(E62="","",IF(E61="",1,1+J61))</f>
         <v/>
       </c>
-      <c r="N62" s="7" t="str">
+      <c r="N62" s="2" t="str">
         <f aca="false">IF(G62="?",_xlfn.CONCAT(AQ62,"Q ",AR62,":",TEXT(AS62,"00")),"")</f>
         <v/>
       </c>
@@ -2987,7 +2983,7 @@
         <f aca="false">IF(AT62="","",IF(AT63="",AV62,AT62-AT63))</f>
         <v/>
       </c>
-      <c r="BF62" s="8" t="n">
+      <c r="BF62" s="7" t="n">
         <f aca="false">BE62=AV62</f>
         <v>1</v>
       </c>
@@ -3012,7 +3008,7 @@
         <f aca="false">IF(E63="","",IF(E62="",1,1+J62))</f>
         <v/>
       </c>
-      <c r="N63" s="7" t="str">
+      <c r="N63" s="2" t="str">
         <f aca="false">IF(G63="?",_xlfn.CONCAT(AQ63,"Q ",AR63,":",TEXT(AS63,"00")),"")</f>
         <v/>
       </c>
@@ -3032,7 +3028,7 @@
         <f aca="false">IF(AT63="","",IF(AT64="",AV63,AT63-AT64))</f>
         <v/>
       </c>
-      <c r="BF63" s="8" t="n">
+      <c r="BF63" s="7" t="n">
         <f aca="false">BE63=AV63</f>
         <v>1</v>
       </c>
@@ -3057,7 +3053,7 @@
         <f aca="false">IF(E64="","",IF(E63="",1,1+J63))</f>
         <v/>
       </c>
-      <c r="N64" s="7" t="str">
+      <c r="N64" s="2" t="str">
         <f aca="false">IF(G64="?",_xlfn.CONCAT(AQ64,"Q ",AR64,":",TEXT(AS64,"00")),"")</f>
         <v/>
       </c>
@@ -3077,7 +3073,7 @@
         <f aca="false">IF(AT64="","",IF(AT65="",AV64,AT64-AT65))</f>
         <v/>
       </c>
-      <c r="BF64" s="8" t="n">
+      <c r="BF64" s="7" t="n">
         <f aca="false">BE64=AV64</f>
         <v>1</v>
       </c>
@@ -3102,7 +3098,7 @@
         <f aca="false">IF(E65="","",IF(E64="",1,1+J64))</f>
         <v/>
       </c>
-      <c r="N65" s="7" t="str">
+      <c r="N65" s="2" t="str">
         <f aca="false">IF(G65="?",_xlfn.CONCAT(AQ65,"Q ",AR65,":",TEXT(AS65,"00")),"")</f>
         <v/>
       </c>
@@ -3122,7 +3118,7 @@
         <f aca="false">IF(AT65="","",IF(AT66="",AV65,AT65-AT66))</f>
         <v/>
       </c>
-      <c r="BF65" s="8" t="n">
+      <c r="BF65" s="7" t="n">
         <f aca="false">BE65=AV65</f>
         <v>1</v>
       </c>
@@ -3147,7 +3143,7 @@
         <f aca="false">IF(E66="","",IF(E65="",1,1+J65))</f>
         <v/>
       </c>
-      <c r="N66" s="7" t="str">
+      <c r="N66" s="2" t="str">
         <f aca="false">IF(G66="?",_xlfn.CONCAT(AQ66,"Q ",AR66,":",TEXT(AS66,"00")),"")</f>
         <v/>
       </c>
@@ -3167,7 +3163,7 @@
         <f aca="false">IF(AT66="","",IF(AT67="",AV66,AT66-AT67))</f>
         <v/>
       </c>
-      <c r="BF66" s="8" t="n">
+      <c r="BF66" s="7" t="n">
         <f aca="false">BE66=AV66</f>
         <v>1</v>
       </c>
@@ -3192,7 +3188,7 @@
         <f aca="false">IF(E67="","",IF(E66="",1,1+J66))</f>
         <v/>
       </c>
-      <c r="N67" s="7" t="str">
+      <c r="N67" s="2" t="str">
         <f aca="false">IF(G67="?",_xlfn.CONCAT(AQ67,"Q ",AR67,":",TEXT(AS67,"00")),"")</f>
         <v/>
       </c>
@@ -3212,7 +3208,7 @@
         <f aca="false">IF(AT67="","",IF(AT68="",AV67,AT67-AT68))</f>
         <v/>
       </c>
-      <c r="BF67" s="8" t="n">
+      <c r="BF67" s="7" t="n">
         <f aca="false">BE67=AV67</f>
         <v>1</v>
       </c>
@@ -3237,7 +3233,7 @@
         <f aca="false">IF(E68="","",IF(E67="",1,1+J67))</f>
         <v/>
       </c>
-      <c r="N68" s="7" t="str">
+      <c r="N68" s="2" t="str">
         <f aca="false">IF(G68="?",_xlfn.CONCAT(AQ68,"Q ",AR68,":",TEXT(AS68,"00")),"")</f>
         <v/>
       </c>
@@ -3257,7 +3253,7 @@
         <f aca="false">IF(AT68="","",IF(AT69="",AV68,AT68-AT69))</f>
         <v/>
       </c>
-      <c r="BF68" s="8" t="n">
+      <c r="BF68" s="7" t="n">
         <f aca="false">BE68=AV68</f>
         <v>1</v>
       </c>
@@ -3282,7 +3278,7 @@
         <f aca="false">IF(E69="","",IF(E68="",1,1+J68))</f>
         <v/>
       </c>
-      <c r="N69" s="7" t="str">
+      <c r="N69" s="2" t="str">
         <f aca="false">IF(G69="?",_xlfn.CONCAT(AQ69,"Q ",AR69,":",TEXT(AS69,"00")),"")</f>
         <v/>
       </c>
@@ -3302,7 +3298,7 @@
         <f aca="false">IF(AT69="","",IF(AT70="",AV69,AT69-AT70))</f>
         <v/>
       </c>
-      <c r="BF69" s="8" t="n">
+      <c r="BF69" s="7" t="n">
         <f aca="false">BE69=AV69</f>
         <v>1</v>
       </c>
@@ -3327,7 +3323,7 @@
         <f aca="false">IF(E70="","",IF(E69="",1,1+J69))</f>
         <v/>
       </c>
-      <c r="N70" s="7" t="str">
+      <c r="N70" s="2" t="str">
         <f aca="false">IF(G70="?",_xlfn.CONCAT(AQ70,"Q ",AR70,":",TEXT(AS70,"00")),"")</f>
         <v/>
       </c>
@@ -3347,7 +3343,7 @@
         <f aca="false">IF(AT70="","",IF(AT71="",AV70,AT70-AT71))</f>
         <v/>
       </c>
-      <c r="BF70" s="8" t="n">
+      <c r="BF70" s="7" t="n">
         <f aca="false">BE70=AV70</f>
         <v>1</v>
       </c>
@@ -3372,7 +3368,7 @@
         <f aca="false">IF(E71="","",IF(E70="",1,1+J70))</f>
         <v/>
       </c>
-      <c r="N71" s="7" t="str">
+      <c r="N71" s="2" t="str">
         <f aca="false">IF(G71="?",_xlfn.CONCAT(AQ71,"Q ",AR71,":",TEXT(AS71,"00")),"")</f>
         <v/>
       </c>
@@ -3392,7 +3388,7 @@
         <f aca="false">IF(AT71="","",IF(AT72="",AV71,AT71-AT72))</f>
         <v/>
       </c>
-      <c r="BF71" s="8" t="n">
+      <c r="BF71" s="7" t="n">
         <f aca="false">BE71=AV71</f>
         <v>1</v>
       </c>
@@ -3417,7 +3413,7 @@
         <f aca="false">IF(E72="","",IF(E71="",1,1+J71))</f>
         <v/>
       </c>
-      <c r="N72" s="7" t="str">
+      <c r="N72" s="2" t="str">
         <f aca="false">IF(G72="?",_xlfn.CONCAT(AQ72,"Q ",AR72,":",TEXT(AS72,"00")),"")</f>
         <v/>
       </c>
@@ -3437,7 +3433,7 @@
         <f aca="false">IF(AT72="","",IF(AT73="",AV72,AT72-AT73))</f>
         <v/>
       </c>
-      <c r="BF72" s="8" t="n">
+      <c r="BF72" s="7" t="n">
         <f aca="false">BE72=AV72</f>
         <v>1</v>
       </c>
@@ -3462,7 +3458,7 @@
         <f aca="false">IF(E73="","",IF(E72="",1,1+J72))</f>
         <v/>
       </c>
-      <c r="N73" s="7" t="str">
+      <c r="N73" s="2" t="str">
         <f aca="false">IF(G73="?",_xlfn.CONCAT(AQ73,"Q ",AR73,":",TEXT(AS73,"00")),"")</f>
         <v/>
       </c>
@@ -3483,7 +3479,7 @@
         <f aca="false">IF(AT73="","",IF(AT74="",AV73,AT73-AT74))</f>
         <v/>
       </c>
-      <c r="BF73" s="8" t="n">
+      <c r="BF73" s="7" t="n">
         <f aca="false">BE73=AV73</f>
         <v>1</v>
       </c>
@@ -3508,7 +3504,7 @@
         <f aca="false">IF(E74="","",IF(E73="",1,1+J73))</f>
         <v/>
       </c>
-      <c r="N74" s="7" t="str">
+      <c r="N74" s="2" t="str">
         <f aca="false">IF(G74="?",_xlfn.CONCAT(AQ74,"Q ",AR74,":",TEXT(AS74,"00")),"")</f>
         <v/>
       </c>
@@ -3529,7 +3525,7 @@
         <f aca="false">IF(AT74="","",IF(AT75="",AV74,AT74-AT75))</f>
         <v/>
       </c>
-      <c r="BF74" s="8" t="n">
+      <c r="BF74" s="7" t="n">
         <f aca="false">BE74=AV74</f>
         <v>1</v>
       </c>
@@ -3554,7 +3550,7 @@
         <f aca="false">IF(E75="","",IF(E74="",1,1+J74))</f>
         <v/>
       </c>
-      <c r="N75" s="7" t="str">
+      <c r="N75" s="2" t="str">
         <f aca="false">IF(G75="?",_xlfn.CONCAT(AQ75,"Q ",AR75,":",TEXT(AS75,"00")),"")</f>
         <v/>
       </c>
@@ -3575,7 +3571,7 @@
         <f aca="false">IF(AT75="","",IF(AT76="",AV75,AT75-AT76))</f>
         <v/>
       </c>
-      <c r="BF75" s="8" t="n">
+      <c r="BF75" s="7" t="n">
         <f aca="false">BE75=AV75</f>
         <v>1</v>
       </c>
@@ -3600,7 +3596,7 @@
         <f aca="false">IF(E76="","",IF(E75="",1,1+J75))</f>
         <v/>
       </c>
-      <c r="N76" s="7" t="str">
+      <c r="N76" s="2" t="str">
         <f aca="false">IF(G76="?",_xlfn.CONCAT(AQ76,"Q ",AR76,":",TEXT(AS76,"00")),"")</f>
         <v/>
       </c>
@@ -3621,7 +3617,7 @@
         <f aca="false">IF(AT76="","",IF(AT77="",AV76,AT76-AT77))</f>
         <v/>
       </c>
-      <c r="BF76" s="8" t="n">
+      <c r="BF76" s="7" t="n">
         <f aca="false">BE76=AV76</f>
         <v>1</v>
       </c>
@@ -3646,7 +3642,7 @@
         <f aca="false">IF(E77="","",IF(E76="",1,1+J76))</f>
         <v/>
       </c>
-      <c r="N77" s="7" t="str">
+      <c r="N77" s="2" t="str">
         <f aca="false">IF(G77="?",_xlfn.CONCAT(AQ77,"Q ",AR77,":",TEXT(AS77,"00")),"")</f>
         <v/>
       </c>
@@ -3667,7 +3663,7 @@
         <f aca="false">IF(AT77="","",IF(AT78="",AV77,AT77-AT78))</f>
         <v/>
       </c>
-      <c r="BF77" s="8" t="n">
+      <c r="BF77" s="7" t="n">
         <f aca="false">BE77=AV77</f>
         <v>1</v>
       </c>
@@ -3692,7 +3688,7 @@
         <f aca="false">IF(E78="","",IF(E77="",1,1+J77))</f>
         <v/>
       </c>
-      <c r="N78" s="7" t="str">
+      <c r="N78" s="2" t="str">
         <f aca="false">IF(G78="?",_xlfn.CONCAT(AQ78,"Q ",AR78,":",TEXT(AS78,"00")),"")</f>
         <v/>
       </c>
@@ -3713,7 +3709,7 @@
         <f aca="false">IF(AT78="","",IF(AT79="",AV78,AT78-AT79))</f>
         <v/>
       </c>
-      <c r="BF78" s="8" t="n">
+      <c r="BF78" s="7" t="n">
         <f aca="false">BE78=AV78</f>
         <v>1</v>
       </c>
@@ -3738,7 +3734,7 @@
         <f aca="false">IF(E79="","",IF(E78="",1,1+J78))</f>
         <v/>
       </c>
-      <c r="N79" s="7" t="str">
+      <c r="N79" s="2" t="str">
         <f aca="false">IF(G79="?",_xlfn.CONCAT(AQ79,"Q ",AR79,":",TEXT(AS79,"00")),"")</f>
         <v/>
       </c>
@@ -3759,7 +3755,7 @@
         <f aca="false">IF(AT79="","",IF(AT80="",AV79,AT79-AT80))</f>
         <v/>
       </c>
-      <c r="BF79" s="8" t="n">
+      <c r="BF79" s="7" t="n">
         <f aca="false">BE79=AV79</f>
         <v>1</v>
       </c>
@@ -3784,7 +3780,7 @@
         <f aca="false">IF(E80="","",IF(E79="",1,1+J79))</f>
         <v/>
       </c>
-      <c r="N80" s="7" t="str">
+      <c r="N80" s="2" t="str">
         <f aca="false">IF(G80="?",_xlfn.CONCAT(AQ80,"Q ",AR80,":",TEXT(AS80,"00")),"")</f>
         <v/>
       </c>
@@ -3805,7 +3801,7 @@
         <f aca="false">IF(AT80="","",IF(AT81="",AV80,AT80-AT81))</f>
         <v/>
       </c>
-      <c r="BF80" s="8" t="n">
+      <c r="BF80" s="7" t="n">
         <f aca="false">BE80=AV80</f>
         <v>1</v>
       </c>
@@ -3830,7 +3826,7 @@
         <f aca="false">IF(E81="","",IF(E80="",1,1+J80))</f>
         <v/>
       </c>
-      <c r="N81" s="7" t="str">
+      <c r="N81" s="2" t="str">
         <f aca="false">IF(G81="?",_xlfn.CONCAT(AQ81,"Q ",AR81,":",TEXT(AS81,"00")),"")</f>
         <v/>
       </c>
@@ -3851,7 +3847,7 @@
         <f aca="false">IF(AT81="","",IF(AT82="",AV81,AT81-AT82))</f>
         <v/>
       </c>
-      <c r="BF81" s="8" t="n">
+      <c r="BF81" s="7" t="n">
         <f aca="false">BE81=AV81</f>
         <v>1</v>
       </c>
@@ -3876,7 +3872,7 @@
         <f aca="false">IF(E82="","",IF(E81="",1,1+J81))</f>
         <v/>
       </c>
-      <c r="N82" s="7" t="str">
+      <c r="N82" s="2" t="str">
         <f aca="false">IF(G82="?",_xlfn.CONCAT(AQ82,"Q ",AR82,":",TEXT(AS82,"00")),"")</f>
         <v/>
       </c>
@@ -3897,7 +3893,7 @@
         <f aca="false">IF(AT82="","",IF(AT83="",AV82,AT82-AT83))</f>
         <v/>
       </c>
-      <c r="BF82" s="8" t="n">
+      <c r="BF82" s="7" t="n">
         <f aca="false">BE82=AV82</f>
         <v>1</v>
       </c>
@@ -3922,7 +3918,7 @@
         <f aca="false">IF(E83="","",IF(E82="",1,1+J82))</f>
         <v/>
       </c>
-      <c r="N83" s="7" t="str">
+      <c r="N83" s="2" t="str">
         <f aca="false">IF(G83="?",_xlfn.CONCAT(AQ83,"Q ",AR83,":",TEXT(AS83,"00")),"")</f>
         <v/>
       </c>
@@ -3943,7 +3939,7 @@
         <f aca="false">IF(AT83="","",IF(AT84="",AV83,AT83-AT84))</f>
         <v/>
       </c>
-      <c r="BF83" s="8" t="n">
+      <c r="BF83" s="7" t="n">
         <f aca="false">BE83=AV83</f>
         <v>1</v>
       </c>
@@ -3968,7 +3964,7 @@
         <f aca="false">IF(E84="","",IF(E83="",1,1+J83))</f>
         <v/>
       </c>
-      <c r="N84" s="7" t="str">
+      <c r="N84" s="2" t="str">
         <f aca="false">IF(G84="?",_xlfn.CONCAT(AQ84,"Q ",AR84,":",TEXT(AS84,"00")),"")</f>
         <v/>
       </c>
@@ -3989,7 +3985,7 @@
         <f aca="false">IF(AT84="","",IF(AT85="",AV84,AT84-AT85))</f>
         <v/>
       </c>
-      <c r="BF84" s="8" t="n">
+      <c r="BF84" s="7" t="n">
         <f aca="false">BE84=AV84</f>
         <v>1</v>
       </c>
@@ -4014,7 +4010,7 @@
         <f aca="false">IF(E85="","",IF(E84="",1,1+J84))</f>
         <v/>
       </c>
-      <c r="N85" s="7" t="str">
+      <c r="N85" s="2" t="str">
         <f aca="false">IF(G85="?",_xlfn.CONCAT(AQ85,"Q ",AR85,":",TEXT(AS85,"00")),"")</f>
         <v/>
       </c>
@@ -4035,7 +4031,7 @@
         <f aca="false">IF(AT85="","",IF(AT86="",AV85,AT85-AT86))</f>
         <v/>
       </c>
-      <c r="BF85" s="8" t="n">
+      <c r="BF85" s="7" t="n">
         <f aca="false">BE85=AV85</f>
         <v>1</v>
       </c>
@@ -4060,7 +4056,7 @@
         <f aca="false">IF(E86="","",IF(E85="",1,1+J85))</f>
         <v/>
       </c>
-      <c r="N86" s="7" t="str">
+      <c r="N86" s="2" t="str">
         <f aca="false">IF(G86="?",_xlfn.CONCAT(AQ86,"Q ",AR86,":",TEXT(AS86,"00")),"")</f>
         <v/>
       </c>
@@ -4080,7 +4076,7 @@
         <f aca="false">IF(AT86="","",IF(AT87="",AV86,AT86-AT87))</f>
         <v/>
       </c>
-      <c r="BF86" s="8" t="n">
+      <c r="BF86" s="7" t="n">
         <f aca="false">BE86=AV86</f>
         <v>1</v>
       </c>
@@ -4105,7 +4101,7 @@
         <f aca="false">IF(E87="","",IF(E86="",1,1+J86))</f>
         <v/>
       </c>
-      <c r="N87" s="7" t="str">
+      <c r="N87" s="2" t="str">
         <f aca="false">IF(G87="?",_xlfn.CONCAT(AQ87,"Q ",AR87,":",TEXT(AS87,"00")),"")</f>
         <v/>
       </c>
@@ -4125,7 +4121,7 @@
         <f aca="false">IF(AT87="","",IF(AT88="",AV87,AT87-AT88))</f>
         <v/>
       </c>
-      <c r="BF87" s="8" t="n">
+      <c r="BF87" s="7" t="n">
         <f aca="false">BE87=AV87</f>
         <v>1</v>
       </c>
@@ -4150,7 +4146,7 @@
         <f aca="false">IF(E88="","",IF(E87="",1,1+J87))</f>
         <v/>
       </c>
-      <c r="N88" s="7" t="str">
+      <c r="N88" s="2" t="str">
         <f aca="false">IF(G88="?",_xlfn.CONCAT(AQ88,"Q ",AR88,":",TEXT(AS88,"00")),"")</f>
         <v/>
       </c>
@@ -4170,7 +4166,7 @@
         <f aca="false">IF(AT88="","",IF(AT89="",AV88,AT88-AT89))</f>
         <v/>
       </c>
-      <c r="BF88" s="8" t="n">
+      <c r="BF88" s="7" t="n">
         <f aca="false">BE88=AV88</f>
         <v>1</v>
       </c>
@@ -4195,7 +4191,7 @@
         <f aca="false">IF(E89="","",IF(E88="",1,1+J88))</f>
         <v/>
       </c>
-      <c r="N89" s="7" t="str">
+      <c r="N89" s="2" t="str">
         <f aca="false">IF(G89="?",_xlfn.CONCAT(AQ89,"Q ",AR89,":",TEXT(AS89,"00")),"")</f>
         <v/>
       </c>
@@ -4215,7 +4211,7 @@
         <f aca="false">IF(AT89="","",IF(AT90="",AV89,AT89-AT90))</f>
         <v/>
       </c>
-      <c r="BF89" s="8" t="n">
+      <c r="BF89" s="7" t="n">
         <f aca="false">BE89=AV89</f>
         <v>1</v>
       </c>
@@ -4240,7 +4236,7 @@
         <f aca="false">IF(E90="","",IF(E89="",1,1+J89))</f>
         <v/>
       </c>
-      <c r="N90" s="7" t="str">
+      <c r="N90" s="2" t="str">
         <f aca="false">IF(G90="?",_xlfn.CONCAT(AQ90,"Q ",AR90,":",TEXT(AS90,"00")),"")</f>
         <v/>
       </c>
@@ -4260,7 +4256,7 @@
         <f aca="false">IF(AT90="","",IF(AT91="",AV90,AT90-AT91))</f>
         <v/>
       </c>
-      <c r="BF90" s="8" t="n">
+      <c r="BF90" s="7" t="n">
         <f aca="false">BE90=AV90</f>
         <v>1</v>
       </c>
@@ -4285,7 +4281,7 @@
         <f aca="false">IF(E91="","",IF(E90="",1,1+J90))</f>
         <v/>
       </c>
-      <c r="N91" s="7" t="str">
+      <c r="N91" s="2" t="str">
         <f aca="false">IF(G91="?",_xlfn.CONCAT(AQ91,"Q ",AR91,":",TEXT(AS91,"00")),"")</f>
         <v/>
       </c>
@@ -4305,7 +4301,7 @@
         <f aca="false">IF(AT91="","",IF(AT92="",AV91,AT91-AT92))</f>
         <v/>
       </c>
-      <c r="BF91" s="8" t="n">
+      <c r="BF91" s="7" t="n">
         <f aca="false">BE91=AV91</f>
         <v>1</v>
       </c>
@@ -4330,7 +4326,7 @@
         <f aca="false">IF(E92="","",IF(E91="",1,1+J91))</f>
         <v/>
       </c>
-      <c r="N92" s="7" t="str">
+      <c r="N92" s="2" t="str">
         <f aca="false">IF(G92="?",_xlfn.CONCAT(AQ92,"Q ",AR92,":",TEXT(AS92,"00")),"")</f>
         <v/>
       </c>
@@ -4350,7 +4346,7 @@
         <f aca="false">IF(AT92="","",IF(AT93="",AV92,AT92-AT93))</f>
         <v/>
       </c>
-      <c r="BF92" s="8" t="n">
+      <c r="BF92" s="7" t="n">
         <f aca="false">BE92=AV92</f>
         <v>1</v>
       </c>
@@ -4375,7 +4371,7 @@
         <f aca="false">IF(E93="","",IF(E92="",1,1+J92))</f>
         <v/>
       </c>
-      <c r="N93" s="7" t="str">
+      <c r="N93" s="2" t="str">
         <f aca="false">IF(G93="?",_xlfn.CONCAT(AQ93,"Q ",AR93,":",TEXT(AS93,"00")),"")</f>
         <v/>
       </c>
@@ -4395,7 +4391,7 @@
         <f aca="false">IF(AT93="","",IF(AT94="",AV93,AT93-AT94))</f>
         <v/>
       </c>
-      <c r="BF93" s="8" t="n">
+      <c r="BF93" s="7" t="n">
         <f aca="false">BE93=AV93</f>
         <v>1</v>
       </c>
@@ -4420,7 +4416,7 @@
         <f aca="false">IF(E94="","",IF(E93="",1,1+J93))</f>
         <v/>
       </c>
-      <c r="N94" s="7" t="str">
+      <c r="N94" s="2" t="str">
         <f aca="false">IF(G94="?",_xlfn.CONCAT(AQ94,"Q ",AR94,":",TEXT(AS94,"00")),"")</f>
         <v/>
       </c>
@@ -4440,7 +4436,7 @@
         <f aca="false">IF(AT94="","",IF(AT95="",AV94,AT94-AT95))</f>
         <v/>
       </c>
-      <c r="BF94" s="8" t="n">
+      <c r="BF94" s="7" t="n">
         <f aca="false">BE94=AV94</f>
         <v>1</v>
       </c>
@@ -4465,7 +4461,7 @@
         <f aca="false">IF(E95="","",IF(E94="",1,1+J94))</f>
         <v/>
       </c>
-      <c r="N95" s="7" t="str">
+      <c r="N95" s="2" t="str">
         <f aca="false">IF(G95="?",_xlfn.CONCAT(AQ95,"Q ",AR95,":",TEXT(AS95,"00")),"")</f>
         <v/>
       </c>
@@ -4485,7 +4481,7 @@
         <f aca="false">IF(AT95="","",IF(AT96="",AV95,AT95-AT96))</f>
         <v/>
       </c>
-      <c r="BF95" s="8" t="n">
+      <c r="BF95" s="7" t="n">
         <f aca="false">BE95=AV95</f>
         <v>1</v>
       </c>
@@ -4510,7 +4506,7 @@
         <f aca="false">IF(E96="","",IF(E95="",1,1+J95))</f>
         <v/>
       </c>
-      <c r="N96" s="7" t="str">
+      <c r="N96" s="2" t="str">
         <f aca="false">IF(G96="?",_xlfn.CONCAT(AQ96,"Q ",AR96,":",TEXT(AS96,"00")),"")</f>
         <v/>
       </c>
@@ -4530,7 +4526,7 @@
         <f aca="false">IF(AT96="","",IF(AT97="",AV96,AT96-AT97))</f>
         <v/>
       </c>
-      <c r="BF96" s="8" t="n">
+      <c r="BF96" s="7" t="n">
         <f aca="false">BE96=AV96</f>
         <v>1</v>
       </c>
@@ -4555,7 +4551,7 @@
         <f aca="false">IF(E97="","",IF(E96="",1,1+J96))</f>
         <v/>
       </c>
-      <c r="N97" s="7" t="str">
+      <c r="N97" s="2" t="str">
         <f aca="false">IF(G97="?",_xlfn.CONCAT(AQ97,"Q ",AR97,":",TEXT(AS97,"00")),"")</f>
         <v/>
       </c>
@@ -4575,7 +4571,7 @@
         <f aca="false">IF(AT97="","",IF(AT98="",AV97,AT97-AT98))</f>
         <v/>
       </c>
-      <c r="BF97" s="8" t="n">
+      <c r="BF97" s="7" t="n">
         <f aca="false">BE97=AV97</f>
         <v>1</v>
       </c>
@@ -4600,7 +4596,7 @@
         <f aca="false">IF(E98="","",IF(E97="",1,1+J97))</f>
         <v/>
       </c>
-      <c r="N98" s="7" t="str">
+      <c r="N98" s="2" t="str">
         <f aca="false">IF(G98="?",_xlfn.CONCAT(AQ98,"Q ",AR98,":",TEXT(AS98,"00")),"")</f>
         <v/>
       </c>
@@ -4620,7 +4616,7 @@
         <f aca="false">IF(AT98="","",IF(AT99="",AV98,AT98-AT99))</f>
         <v/>
       </c>
-      <c r="BF98" s="8" t="n">
+      <c r="BF98" s="7" t="n">
         <f aca="false">BE98=AV98</f>
         <v>1</v>
       </c>
@@ -4645,7 +4641,7 @@
         <f aca="false">IF(E99="","",IF(E98="",1,1+J98))</f>
         <v/>
       </c>
-      <c r="N99" s="7" t="str">
+      <c r="N99" s="2" t="str">
         <f aca="false">IF(G99="?",_xlfn.CONCAT(AQ99,"Q ",AR99,":",TEXT(AS99,"00")),"")</f>
         <v/>
       </c>
@@ -4665,7 +4661,7 @@
         <f aca="false">IF(AT99="","",IF(AT100="",AV99,AT99-AT100))</f>
         <v/>
       </c>
-      <c r="BF99" s="8" t="n">
+      <c r="BF99" s="7" t="n">
         <f aca="false">BE99=AV99</f>
         <v>1</v>
       </c>
@@ -4690,7 +4686,7 @@
         <f aca="false">IF(E100="","",IF(E99="",1,1+J99))</f>
         <v/>
       </c>
-      <c r="N100" s="7" t="str">
+      <c r="N100" s="2" t="str">
         <f aca="false">IF(G100="?",_xlfn.CONCAT(AQ100,"Q ",AR100,":",TEXT(AS100,"00")),"")</f>
         <v/>
       </c>
@@ -4710,7 +4706,7 @@
         <f aca="false">IF(AT100="","",IF(AT101="",AV100,AT100-AT101))</f>
         <v/>
       </c>
-      <c r="BF100" s="8" t="n">
+      <c r="BF100" s="7" t="n">
         <f aca="false">BE100=AV100</f>
         <v>1</v>
       </c>
@@ -4733,10 +4729,10 @@
   </sheetPr>
   <dimension ref="C1:BF100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="11" ySplit="0" topLeftCell="AY70" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
-      <selection pane="topRight" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="11" ySplit="0" topLeftCell="AY1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="BK4" activeCellId="0" sqref="BK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4769,7 +4765,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="2.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="44" style="1" width="3.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="3.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="4.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="4.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="155.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="51" style="1" width="3.51"/>
@@ -4793,7 +4789,7 @@
       <c r="J1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N1" s="7" t="str">
+      <c r="N1" s="2" t="str">
         <f aca="false">IF(G1="?",_xlfn.CONCAT(AQ1,"Q ",AR1,":",TEXT(AS1,"00")),"")</f>
         <v/>
       </c>
@@ -4813,7 +4809,7 @@
         <f aca="false">IF(AT1="","",IF(AT2="",AV1,AT1-AT2))</f>
         <v/>
       </c>
-      <c r="BF1" s="8" t="n">
+      <c r="BF1" s="7" t="n">
         <f aca="false">BE1=AV1</f>
         <v>1</v>
       </c>
@@ -4837,7 +4833,7 @@
         <f aca="false">IF(E2="","",IF(E1="",1,1+J1))</f>
         <v/>
       </c>
-      <c r="N2" s="7" t="str">
+      <c r="N2" s="2" t="str">
         <f aca="false">IF(G2="?",_xlfn.CONCAT(AQ2,"Q ",AR2,":",TEXT(AS2,"00")),"")</f>
         <v/>
       </c>
@@ -4857,7 +4853,7 @@
         <f aca="false">IF(AT2="","",IF(AT3="",AV2,AT2-AT3))</f>
         <v/>
       </c>
-      <c r="BF2" s="8" t="n">
+      <c r="BF2" s="7" t="n">
         <f aca="false">BE2=AV2</f>
         <v>1</v>
       </c>
@@ -4882,7 +4878,7 @@
         <f aca="false">IF(E3="","",IF(E2="",1,1+J2))</f>
         <v/>
       </c>
-      <c r="N3" s="7" t="str">
+      <c r="N3" s="2" t="str">
         <f aca="false">IF(G3="?",_xlfn.CONCAT(AQ3,"Q ",AR3,":",TEXT(AS3,"00")),"")</f>
         <v/>
       </c>
@@ -4902,7 +4898,7 @@
         <f aca="false">IF(AT3="","",IF(AT4="",AV3,AT3-AT4))</f>
         <v/>
       </c>
-      <c r="BF3" s="8" t="n">
+      <c r="BF3" s="7" t="n">
         <f aca="false">BE3=AV3</f>
         <v>1</v>
       </c>
@@ -4927,7 +4923,7 @@
         <f aca="false">IF(E4="","",IF(E3="",1,1+J3))</f>
         <v/>
       </c>
-      <c r="N4" s="7" t="str">
+      <c r="N4" s="2" t="str">
         <f aca="false">IF(G4="?",_xlfn.CONCAT(AQ4,"Q ",AR4,":",TEXT(AS4,"00")),"")</f>
         <v/>
       </c>
@@ -4947,7 +4943,7 @@
         <f aca="false">IF(AT4="","",IF(AT5="",AV4,AT4-AT5))</f>
         <v/>
       </c>
-      <c r="BF4" s="8" t="n">
+      <c r="BF4" s="7" t="n">
         <f aca="false">BE4=AV4</f>
         <v>1</v>
       </c>
@@ -4972,7 +4968,7 @@
         <f aca="false">IF(E5="","",IF(E4="",1,1+J4))</f>
         <v/>
       </c>
-      <c r="N5" s="7" t="str">
+      <c r="N5" s="2" t="str">
         <f aca="false">IF(G5="?",_xlfn.CONCAT(AQ5,"Q ",AR5,":",TEXT(AS5,"00")),"")</f>
         <v/>
       </c>
@@ -4992,7 +4988,7 @@
         <f aca="false">IF(AT5="","",IF(AT6="",AV5,AT5-AT6))</f>
         <v/>
       </c>
-      <c r="BF5" s="8" t="n">
+      <c r="BF5" s="7" t="n">
         <f aca="false">BE5=AV5</f>
         <v>1</v>
       </c>
@@ -5017,7 +5013,7 @@
         <f aca="false">IF(E6="","",IF(E5="",1,1+J5))</f>
         <v/>
       </c>
-      <c r="N6" s="7" t="str">
+      <c r="N6" s="2" t="str">
         <f aca="false">IF(G6="?",_xlfn.CONCAT(AQ6,"Q ",AR6,":",TEXT(AS6,"00")),"")</f>
         <v/>
       </c>
@@ -5037,7 +5033,7 @@
         <f aca="false">IF(AT6="","",IF(AT7="",AV6,AT6-AT7))</f>
         <v/>
       </c>
-      <c r="BF6" s="8" t="n">
+      <c r="BF6" s="7" t="n">
         <f aca="false">BE6=AV6</f>
         <v>1</v>
       </c>
@@ -5062,7 +5058,7 @@
         <f aca="false">IF(E7="","",IF(E6="",1,1+J6))</f>
         <v/>
       </c>
-      <c r="N7" s="7" t="str">
+      <c r="N7" s="2" t="str">
         <f aca="false">IF(G7="?",_xlfn.CONCAT(AQ7,"Q ",AR7,":",TEXT(AS7,"00")),"")</f>
         <v/>
       </c>
@@ -5082,7 +5078,7 @@
         <f aca="false">IF(AT7="","",IF(AT8="",AV7,AT7-AT8))</f>
         <v/>
       </c>
-      <c r="BF7" s="8" t="n">
+      <c r="BF7" s="7" t="n">
         <f aca="false">BE7=AV7</f>
         <v>1</v>
       </c>
@@ -5107,7 +5103,7 @@
         <f aca="false">IF(E8="","",IF(E7="",1,1+J7))</f>
         <v/>
       </c>
-      <c r="N8" s="7" t="str">
+      <c r="N8" s="2" t="str">
         <f aca="false">IF(G8="?",_xlfn.CONCAT(AQ8,"Q ",AR8,":",TEXT(AS8,"00")),"")</f>
         <v/>
       </c>
@@ -5127,7 +5123,7 @@
         <f aca="false">IF(AT8="","",IF(AT9="",AV8,AT8-AT9))</f>
         <v/>
       </c>
-      <c r="BF8" s="8" t="n">
+      <c r="BF8" s="7" t="n">
         <f aca="false">BE8=AV8</f>
         <v>1</v>
       </c>
@@ -5152,7 +5148,7 @@
         <f aca="false">IF(E9="","",IF(E8="",1,1+J8))</f>
         <v/>
       </c>
-      <c r="N9" s="7" t="str">
+      <c r="N9" s="2" t="str">
         <f aca="false">IF(G9="?",_xlfn.CONCAT(AQ9,"Q ",AR9,":",TEXT(AS9,"00")),"")</f>
         <v/>
       </c>
@@ -5172,7 +5168,7 @@
         <f aca="false">IF(AT9="","",IF(AT10="",AV9,AT9-AT10))</f>
         <v/>
       </c>
-      <c r="BF9" s="8" t="n">
+      <c r="BF9" s="7" t="n">
         <f aca="false">BE9=AV9</f>
         <v>1</v>
       </c>
@@ -5197,7 +5193,7 @@
         <f aca="false">IF(E10="","",IF(E9="",1,1+J9))</f>
         <v/>
       </c>
-      <c r="N10" s="7" t="str">
+      <c r="N10" s="2" t="str">
         <f aca="false">IF(G10="?",_xlfn.CONCAT(AQ10,"Q ",AR10,":",TEXT(AS10,"00")),"")</f>
         <v/>
       </c>
@@ -5217,7 +5213,7 @@
         <f aca="false">IF(AT10="","",IF(AT11="",AV10,AT10-AT11))</f>
         <v/>
       </c>
-      <c r="BF10" s="8" t="n">
+      <c r="BF10" s="7" t="n">
         <f aca="false">BE10=AV10</f>
         <v>1</v>
       </c>
@@ -5242,7 +5238,7 @@
         <f aca="false">IF(E11="","",IF(E10="",1,1+J10))</f>
         <v/>
       </c>
-      <c r="N11" s="7" t="str">
+      <c r="N11" s="2" t="str">
         <f aca="false">IF(G11="?",_xlfn.CONCAT(AQ11,"Q ",AR11,":",TEXT(AS11,"00")),"")</f>
         <v/>
       </c>
@@ -5262,7 +5258,7 @@
         <f aca="false">IF(AT11="","",IF(AT12="",AV11,AT11-AT12))</f>
         <v/>
       </c>
-      <c r="BF11" s="8" t="n">
+      <c r="BF11" s="7" t="n">
         <f aca="false">BE11=AV11</f>
         <v>1</v>
       </c>
@@ -5287,7 +5283,7 @@
         <f aca="false">IF(E12="","",IF(E11="",1,1+J11))</f>
         <v/>
       </c>
-      <c r="N12" s="7" t="str">
+      <c r="N12" s="2" t="str">
         <f aca="false">IF(G12="?",_xlfn.CONCAT(AQ12,"Q ",AR12,":",TEXT(AS12,"00")),"")</f>
         <v/>
       </c>
@@ -5307,7 +5303,7 @@
         <f aca="false">IF(AT12="","",IF(AT13="",AV12,AT12-AT13))</f>
         <v/>
       </c>
-      <c r="BF12" s="8" t="n">
+      <c r="BF12" s="7" t="n">
         <f aca="false">BE12=AV12</f>
         <v>1</v>
       </c>
@@ -5332,7 +5328,7 @@
         <f aca="false">IF(E13="","",IF(E12="",1,1+J12))</f>
         <v/>
       </c>
-      <c r="N13" s="7" t="str">
+      <c r="N13" s="2" t="str">
         <f aca="false">IF(G13="?",_xlfn.CONCAT(AQ13,"Q ",AR13,":",TEXT(AS13,"00")),"")</f>
         <v/>
       </c>
@@ -5352,7 +5348,7 @@
         <f aca="false">IF(AT13="","",IF(AT14="",AV13,AT13-AT14))</f>
         <v/>
       </c>
-      <c r="BF13" s="8" t="n">
+      <c r="BF13" s="7" t="n">
         <f aca="false">BE13=AV13</f>
         <v>1</v>
       </c>
@@ -5377,7 +5373,7 @@
         <f aca="false">IF(E14="","",IF(E13="",1,1+J13))</f>
         <v/>
       </c>
-      <c r="N14" s="7" t="str">
+      <c r="N14" s="2" t="str">
         <f aca="false">IF(G14="?",_xlfn.CONCAT(AQ14,"Q ",AR14,":",TEXT(AS14,"00")),"")</f>
         <v/>
       </c>
@@ -5397,7 +5393,7 @@
         <f aca="false">IF(AT14="","",IF(AT15="",AV14,AT14-AT15))</f>
         <v/>
       </c>
-      <c r="BF14" s="8" t="n">
+      <c r="BF14" s="7" t="n">
         <f aca="false">BE14=AV14</f>
         <v>1</v>
       </c>
@@ -5422,7 +5418,7 @@
         <f aca="false">IF(E15="","",IF(E14="",1,1+J14))</f>
         <v/>
       </c>
-      <c r="N15" s="7" t="str">
+      <c r="N15" s="2" t="str">
         <f aca="false">IF(G15="?",_xlfn.CONCAT(AQ15,"Q ",AR15,":",TEXT(AS15,"00")),"")</f>
         <v/>
       </c>
@@ -5442,7 +5438,7 @@
         <f aca="false">IF(AT15="","",IF(AT16="",AV15,AT15-AT16))</f>
         <v/>
       </c>
-      <c r="BF15" s="8" t="n">
+      <c r="BF15" s="7" t="n">
         <f aca="false">BE15=AV15</f>
         <v>1</v>
       </c>
@@ -5467,7 +5463,7 @@
         <f aca="false">IF(E16="","",IF(E15="",1,1+J15))</f>
         <v/>
       </c>
-      <c r="N16" s="7" t="str">
+      <c r="N16" s="2" t="str">
         <f aca="false">IF(G16="?",_xlfn.CONCAT(AQ16,"Q ",AR16,":",TEXT(AS16,"00")),"")</f>
         <v/>
       </c>
@@ -5487,7 +5483,7 @@
         <f aca="false">IF(AT16="","",IF(AT17="",AV16,AT16-AT17))</f>
         <v/>
       </c>
-      <c r="BF16" s="8" t="n">
+      <c r="BF16" s="7" t="n">
         <f aca="false">BE16=AV16</f>
         <v>1</v>
       </c>
@@ -5512,7 +5508,7 @@
         <f aca="false">IF(E17="","",IF(E16="",1,1+J16))</f>
         <v/>
       </c>
-      <c r="N17" s="7" t="str">
+      <c r="N17" s="2" t="str">
         <f aca="false">IF(G17="?",_xlfn.CONCAT(AQ17,"Q ",AR17,":",TEXT(AS17,"00")),"")</f>
         <v/>
       </c>
@@ -5532,7 +5528,7 @@
         <f aca="false">IF(AT17="","",IF(AT18="",AV17,AT17-AT18))</f>
         <v/>
       </c>
-      <c r="BF17" s="8" t="n">
+      <c r="BF17" s="7" t="n">
         <f aca="false">BE17=AV17</f>
         <v>1</v>
       </c>
@@ -5557,7 +5553,7 @@
         <f aca="false">IF(E18="","",IF(E17="",1,1+J17))</f>
         <v/>
       </c>
-      <c r="N18" s="7" t="str">
+      <c r="N18" s="2" t="str">
         <f aca="false">IF(G18="?",_xlfn.CONCAT(AQ18,"Q ",AR18,":",TEXT(AS18,"00")),"")</f>
         <v/>
       </c>
@@ -5577,7 +5573,7 @@
         <f aca="false">IF(AT18="","",IF(AT19="",AV18,AT18-AT19))</f>
         <v/>
       </c>
-      <c r="BF18" s="8" t="n">
+      <c r="BF18" s="7" t="n">
         <f aca="false">BE18=AV18</f>
         <v>1</v>
       </c>
@@ -5602,7 +5598,7 @@
         <f aca="false">IF(E19="","",IF(E18="",1,1+J18))</f>
         <v/>
       </c>
-      <c r="N19" s="7" t="str">
+      <c r="N19" s="2" t="str">
         <f aca="false">IF(G19="?",_xlfn.CONCAT(AQ19,"Q ",AR19,":",TEXT(AS19,"00")),"")</f>
         <v/>
       </c>
@@ -5622,7 +5618,7 @@
         <f aca="false">IF(AT19="","",IF(AT20="",AV19,AT19-AT20))</f>
         <v/>
       </c>
-      <c r="BF19" s="8" t="n">
+      <c r="BF19" s="7" t="n">
         <f aca="false">BE19=AV19</f>
         <v>1</v>
       </c>
@@ -5647,7 +5643,7 @@
         <f aca="false">IF(E20="","",IF(E19="",1,1+J19))</f>
         <v/>
       </c>
-      <c r="N20" s="7" t="str">
+      <c r="N20" s="2" t="str">
         <f aca="false">IF(G20="?",_xlfn.CONCAT(AQ20,"Q ",AR20,":",TEXT(AS20,"00")),"")</f>
         <v/>
       </c>
@@ -5667,7 +5663,7 @@
         <f aca="false">IF(AT20="","",IF(AT21="",AV20,AT20-AT21))</f>
         <v/>
       </c>
-      <c r="BF20" s="8" t="n">
+      <c r="BF20" s="7" t="n">
         <f aca="false">BE20=AV20</f>
         <v>1</v>
       </c>
@@ -5692,7 +5688,7 @@
         <f aca="false">IF(E21="","",IF(E20="",1,1+J20))</f>
         <v/>
       </c>
-      <c r="N21" s="7" t="str">
+      <c r="N21" s="2" t="str">
         <f aca="false">IF(G21="?",_xlfn.CONCAT(AQ21,"Q ",AR21,":",TEXT(AS21,"00")),"")</f>
         <v/>
       </c>
@@ -5712,7 +5708,7 @@
         <f aca="false">IF(AT21="","",IF(AT22="",AV21,AT21-AT22))</f>
         <v/>
       </c>
-      <c r="BF21" s="8" t="n">
+      <c r="BF21" s="7" t="n">
         <f aca="false">BE21=AV21</f>
         <v>1</v>
       </c>
@@ -5737,7 +5733,7 @@
         <f aca="false">IF(E22="","",IF(E21="",1,1+J21))</f>
         <v/>
       </c>
-      <c r="N22" s="7" t="str">
+      <c r="N22" s="2" t="str">
         <f aca="false">IF(G22="?",_xlfn.CONCAT(AQ22,"Q ",AR22,":",TEXT(AS22,"00")),"")</f>
         <v/>
       </c>
@@ -5757,7 +5753,7 @@
         <f aca="false">IF(AT22="","",IF(AT23="",AV22,AT22-AT23))</f>
         <v/>
       </c>
-      <c r="BF22" s="8" t="n">
+      <c r="BF22" s="7" t="n">
         <f aca="false">BE22=AV22</f>
         <v>1</v>
       </c>
@@ -5782,7 +5778,7 @@
         <f aca="false">IF(E23="","",IF(E22="",1,1+J22))</f>
         <v/>
       </c>
-      <c r="N23" s="7" t="str">
+      <c r="N23" s="2" t="str">
         <f aca="false">IF(G23="?",_xlfn.CONCAT(AQ23,"Q ",AR23,":",TEXT(AS23,"00")),"")</f>
         <v/>
       </c>
@@ -5802,7 +5798,7 @@
         <f aca="false">IF(AT23="","",IF(AT24="",AV23,AT23-AT24))</f>
         <v/>
       </c>
-      <c r="BF23" s="8" t="n">
+      <c r="BF23" s="7" t="n">
         <f aca="false">BE23=AV23</f>
         <v>1</v>
       </c>
@@ -5827,7 +5823,7 @@
         <f aca="false">IF(E24="","",IF(E23="",1,1+J23))</f>
         <v/>
       </c>
-      <c r="N24" s="7" t="str">
+      <c r="N24" s="2" t="str">
         <f aca="false">IF(G24="?",_xlfn.CONCAT(AQ24,"Q ",AR24,":",TEXT(AS24,"00")),"")</f>
         <v/>
       </c>
@@ -5847,7 +5843,7 @@
         <f aca="false">IF(AT24="","",IF(AT25="",AV24,AT24-AT25))</f>
         <v/>
       </c>
-      <c r="BF24" s="8" t="n">
+      <c r="BF24" s="7" t="n">
         <f aca="false">BE24=AV24</f>
         <v>1</v>
       </c>
@@ -5872,7 +5868,7 @@
         <f aca="false">IF(E25="","",IF(E24="",1,1+J24))</f>
         <v/>
       </c>
-      <c r="N25" s="7" t="str">
+      <c r="N25" s="2" t="str">
         <f aca="false">IF(G25="?",_xlfn.CONCAT(AQ25,"Q ",AR25,":",TEXT(AS25,"00")),"")</f>
         <v/>
       </c>
@@ -5892,7 +5888,7 @@
         <f aca="false">IF(AT25="","",IF(AT26="",AV25,AT25-AT26))</f>
         <v/>
       </c>
-      <c r="BF25" s="8" t="n">
+      <c r="BF25" s="7" t="n">
         <f aca="false">BE25=AV25</f>
         <v>1</v>
       </c>
@@ -5917,7 +5913,7 @@
         <f aca="false">IF(E26="","",IF(E25="",1,1+J25))</f>
         <v/>
       </c>
-      <c r="N26" s="7" t="str">
+      <c r="N26" s="2" t="str">
         <f aca="false">IF(G26="?",_xlfn.CONCAT(AQ26,"Q ",AR26,":",TEXT(AS26,"00")),"")</f>
         <v/>
       </c>
@@ -5937,7 +5933,7 @@
         <f aca="false">IF(AT26="","",IF(AT27="",AV26,AT26-AT27))</f>
         <v/>
       </c>
-      <c r="BF26" s="8" t="n">
+      <c r="BF26" s="7" t="n">
         <f aca="false">BE26=AV26</f>
         <v>1</v>
       </c>
@@ -5962,7 +5958,7 @@
         <f aca="false">IF(E27="","",IF(E26="",1,1+J26))</f>
         <v/>
       </c>
-      <c r="N27" s="7" t="str">
+      <c r="N27" s="2" t="str">
         <f aca="false">IF(G27="?",_xlfn.CONCAT(AQ27,"Q ",AR27,":",TEXT(AS27,"00")),"")</f>
         <v/>
       </c>
@@ -5982,7 +5978,7 @@
         <f aca="false">IF(AT27="","",IF(AT28="",AV27,AT27-AT28))</f>
         <v/>
       </c>
-      <c r="BF27" s="8" t="n">
+      <c r="BF27" s="7" t="n">
         <f aca="false">BE27=AV27</f>
         <v>1</v>
       </c>
@@ -6007,7 +6003,7 @@
         <f aca="false">IF(E28="","",IF(E27="",1,1+J27))</f>
         <v/>
       </c>
-      <c r="N28" s="7" t="str">
+      <c r="N28" s="2" t="str">
         <f aca="false">IF(G28="?",_xlfn.CONCAT(AQ28,"Q ",AR28,":",TEXT(AS28,"00")),"")</f>
         <v/>
       </c>
@@ -6027,7 +6023,7 @@
         <f aca="false">IF(AT28="","",IF(AT29="",AV28,AT28-AT29))</f>
         <v/>
       </c>
-      <c r="BF28" s="8" t="n">
+      <c r="BF28" s="7" t="n">
         <f aca="false">BE28=AV28</f>
         <v>1</v>
       </c>
@@ -6052,7 +6048,7 @@
         <f aca="false">IF(E29="","",IF(E28="",1,1+J28))</f>
         <v/>
       </c>
-      <c r="N29" s="7" t="str">
+      <c r="N29" s="2" t="str">
         <f aca="false">IF(G29="?",_xlfn.CONCAT(AQ29,"Q ",AR29,":",TEXT(AS29,"00")),"")</f>
         <v/>
       </c>
@@ -6072,7 +6068,7 @@
         <f aca="false">IF(AT29="","",IF(AT30="",AV29,AT29-AT30))</f>
         <v/>
       </c>
-      <c r="BF29" s="8" t="n">
+      <c r="BF29" s="7" t="n">
         <f aca="false">BE29=AV29</f>
         <v>1</v>
       </c>
@@ -6097,7 +6093,7 @@
         <f aca="false">IF(E30="","",IF(E29="",1,1+J29))</f>
         <v/>
       </c>
-      <c r="N30" s="7" t="str">
+      <c r="N30" s="2" t="str">
         <f aca="false">IF(G30="?",_xlfn.CONCAT(AQ30,"Q ",AR30,":",TEXT(AS30,"00")),"")</f>
         <v/>
       </c>
@@ -6117,7 +6113,7 @@
         <f aca="false">IF(AT30="","",IF(AT31="",AV30,AT30-AT31))</f>
         <v/>
       </c>
-      <c r="BF30" s="8" t="n">
+      <c r="BF30" s="7" t="n">
         <f aca="false">BE30=AV30</f>
         <v>1</v>
       </c>
@@ -6142,7 +6138,7 @@
         <f aca="false">IF(E31="","",IF(E30="",1,1+J30))</f>
         <v/>
       </c>
-      <c r="N31" s="7" t="str">
+      <c r="N31" s="2" t="str">
         <f aca="false">IF(G31="?",_xlfn.CONCAT(AQ31,"Q ",AR31,":",TEXT(AS31,"00")),"")</f>
         <v/>
       </c>
@@ -6162,7 +6158,7 @@
         <f aca="false">IF(AT31="","",IF(AT32="",AV31,AT31-AT32))</f>
         <v/>
       </c>
-      <c r="BF31" s="8" t="n">
+      <c r="BF31" s="7" t="n">
         <f aca="false">BE31=AV31</f>
         <v>1</v>
       </c>
@@ -6187,7 +6183,7 @@
         <f aca="false">IF(E32="","",IF(E31="",1,1+J31))</f>
         <v/>
       </c>
-      <c r="N32" s="7" t="str">
+      <c r="N32" s="2" t="str">
         <f aca="false">IF(G32="?",_xlfn.CONCAT(AQ32,"Q ",AR32,":",TEXT(AS32,"00")),"")</f>
         <v/>
       </c>
@@ -6207,7 +6203,7 @@
         <f aca="false">IF(AT32="","",IF(AT33="",AV32,AT32-AT33))</f>
         <v/>
       </c>
-      <c r="BF32" s="8" t="n">
+      <c r="BF32" s="7" t="n">
         <f aca="false">BE32=AV32</f>
         <v>1</v>
       </c>
@@ -6232,7 +6228,7 @@
         <f aca="false">IF(E33="","",IF(E32="",1,1+J32))</f>
         <v/>
       </c>
-      <c r="N33" s="7" t="str">
+      <c r="N33" s="2" t="str">
         <f aca="false">IF(G33="?",_xlfn.CONCAT(AQ33,"Q ",AR33,":",TEXT(AS33,"00")),"")</f>
         <v/>
       </c>
@@ -6252,7 +6248,7 @@
         <f aca="false">IF(AT33="","",IF(AT34="",AV33,AT33-AT34))</f>
         <v/>
       </c>
-      <c r="BF33" s="8" t="n">
+      <c r="BF33" s="7" t="n">
         <f aca="false">BE33=AV33</f>
         <v>1</v>
       </c>
@@ -6277,7 +6273,7 @@
         <f aca="false">IF(E34="","",IF(E33="",1,1+J33))</f>
         <v/>
       </c>
-      <c r="N34" s="7" t="str">
+      <c r="N34" s="2" t="str">
         <f aca="false">IF(G34="?",_xlfn.CONCAT(AQ34,"Q ",AR34,":",TEXT(AS34,"00")),"")</f>
         <v/>
       </c>
@@ -6297,7 +6293,7 @@
         <f aca="false">IF(AT34="","",IF(AT35="",AV34,AT34-AT35))</f>
         <v/>
       </c>
-      <c r="BF34" s="8" t="n">
+      <c r="BF34" s="7" t="n">
         <f aca="false">BE34=AV34</f>
         <v>1</v>
       </c>
@@ -6322,7 +6318,7 @@
         <f aca="false">IF(E35="","",IF(E34="",1,1+J34))</f>
         <v/>
       </c>
-      <c r="N35" s="7" t="str">
+      <c r="N35" s="2" t="str">
         <f aca="false">IF(G35="?",_xlfn.CONCAT(AQ35,"Q ",AR35,":",TEXT(AS35,"00")),"")</f>
         <v/>
       </c>
@@ -6342,7 +6338,7 @@
         <f aca="false">IF(AT35="","",IF(AT36="",AV35,AT35-AT36))</f>
         <v/>
       </c>
-      <c r="BF35" s="8" t="n">
+      <c r="BF35" s="7" t="n">
         <f aca="false">BE35=AV35</f>
         <v>1</v>
       </c>
@@ -6367,7 +6363,7 @@
         <f aca="false">IF(E36="","",IF(E35="",1,1+J35))</f>
         <v/>
       </c>
-      <c r="N36" s="7" t="str">
+      <c r="N36" s="2" t="str">
         <f aca="false">IF(G36="?",_xlfn.CONCAT(AQ36,"Q ",AR36,":",TEXT(AS36,"00")),"")</f>
         <v/>
       </c>
@@ -6387,7 +6383,7 @@
         <f aca="false">IF(AT36="","",IF(AT37="",AV36,AT36-AT37))</f>
         <v/>
       </c>
-      <c r="BF36" s="8" t="n">
+      <c r="BF36" s="7" t="n">
         <f aca="false">BE36=AV36</f>
         <v>1</v>
       </c>
@@ -6412,7 +6408,7 @@
         <f aca="false">IF(E37="","",IF(E36="",1,1+J36))</f>
         <v/>
       </c>
-      <c r="N37" s="7" t="str">
+      <c r="N37" s="2" t="str">
         <f aca="false">IF(G37="?",_xlfn.CONCAT(AQ37,"Q ",AR37,":",TEXT(AS37,"00")),"")</f>
         <v/>
       </c>
@@ -6432,7 +6428,7 @@
         <f aca="false">IF(AT37="","",IF(AT38="",AV37,AT37-AT38))</f>
         <v/>
       </c>
-      <c r="BF37" s="8" t="n">
+      <c r="BF37" s="7" t="n">
         <f aca="false">BE37=AV37</f>
         <v>1</v>
       </c>
@@ -6457,7 +6453,7 @@
         <f aca="false">IF(E38="","",IF(E37="",1,1+J37))</f>
         <v/>
       </c>
-      <c r="N38" s="7" t="str">
+      <c r="N38" s="2" t="str">
         <f aca="false">IF(G38="?",_xlfn.CONCAT(AQ38,"Q ",AR38,":",TEXT(AS38,"00")),"")</f>
         <v/>
       </c>
@@ -6477,7 +6473,7 @@
         <f aca="false">IF(AT38="","",IF(AT39="",AV38,AT38-AT39))</f>
         <v/>
       </c>
-      <c r="BF38" s="8" t="n">
+      <c r="BF38" s="7" t="n">
         <f aca="false">BE38=AV38</f>
         <v>1</v>
       </c>
@@ -6502,7 +6498,7 @@
         <f aca="false">IF(E39="","",IF(E38="",1,1+J38))</f>
         <v/>
       </c>
-      <c r="N39" s="7" t="str">
+      <c r="N39" s="2" t="str">
         <f aca="false">IF(G39="?",_xlfn.CONCAT(AQ39,"Q ",AR39,":",TEXT(AS39,"00")),"")</f>
         <v/>
       </c>
@@ -6522,7 +6518,7 @@
         <f aca="false">IF(AT39="","",IF(AT40="",AV39,AT39-AT40))</f>
         <v/>
       </c>
-      <c r="BF39" s="8" t="n">
+      <c r="BF39" s="7" t="n">
         <f aca="false">BE39=AV39</f>
         <v>1</v>
       </c>
@@ -6547,7 +6543,7 @@
         <f aca="false">IF(E40="","",IF(E39="",1,1+J39))</f>
         <v/>
       </c>
-      <c r="N40" s="7" t="str">
+      <c r="N40" s="2" t="str">
         <f aca="false">IF(G40="?",_xlfn.CONCAT(AQ40,"Q ",AR40,":",TEXT(AS40,"00")),"")</f>
         <v/>
       </c>
@@ -6567,7 +6563,7 @@
         <f aca="false">IF(AT40="","",IF(AT41="",AV40,AT40-AT41))</f>
         <v/>
       </c>
-      <c r="BF40" s="8" t="n">
+      <c r="BF40" s="7" t="n">
         <f aca="false">BE40=AV40</f>
         <v>1</v>
       </c>
@@ -6592,7 +6588,7 @@
         <f aca="false">IF(E41="","",IF(E40="",1,1+J40))</f>
         <v/>
       </c>
-      <c r="N41" s="7" t="str">
+      <c r="N41" s="2" t="str">
         <f aca="false">IF(G41="?",_xlfn.CONCAT(AQ41,"Q ",AR41,":",TEXT(AS41,"00")),"")</f>
         <v/>
       </c>
@@ -6612,7 +6608,7 @@
         <f aca="false">IF(AT41="","",IF(AT42="",AV41,AT41-AT42))</f>
         <v/>
       </c>
-      <c r="BF41" s="8" t="n">
+      <c r="BF41" s="7" t="n">
         <f aca="false">BE41=AV41</f>
         <v>1</v>
       </c>
@@ -6637,7 +6633,7 @@
         <f aca="false">IF(E42="","",IF(E41="",1,1+J41))</f>
         <v/>
       </c>
-      <c r="N42" s="7" t="str">
+      <c r="N42" s="2" t="str">
         <f aca="false">IF(G42="?",_xlfn.CONCAT(AQ42,"Q ",AR42,":",TEXT(AS42,"00")),"")</f>
         <v/>
       </c>
@@ -6657,7 +6653,7 @@
         <f aca="false">IF(AT42="","",IF(AT43="",AV42,AT42-AT43))</f>
         <v/>
       </c>
-      <c r="BF42" s="8" t="n">
+      <c r="BF42" s="7" t="n">
         <f aca="false">BE42=AV42</f>
         <v>1</v>
       </c>
@@ -6682,7 +6678,7 @@
         <f aca="false">IF(E43="","",IF(E42="",1,1+J42))</f>
         <v/>
       </c>
-      <c r="N43" s="7" t="str">
+      <c r="N43" s="2" t="str">
         <f aca="false">IF(G43="?",_xlfn.CONCAT(AQ43,"Q ",AR43,":",TEXT(AS43,"00")),"")</f>
         <v/>
       </c>
@@ -6702,7 +6698,7 @@
         <f aca="false">IF(AT43="","",IF(AT44="",AV43,AT43-AT44))</f>
         <v/>
       </c>
-      <c r="BF43" s="8" t="n">
+      <c r="BF43" s="7" t="n">
         <f aca="false">BE43=AV43</f>
         <v>1</v>
       </c>
@@ -6727,7 +6723,7 @@
         <f aca="false">IF(E44="","",IF(E43="",1,1+J43))</f>
         <v/>
       </c>
-      <c r="N44" s="7" t="str">
+      <c r="N44" s="2" t="str">
         <f aca="false">IF(G44="?",_xlfn.CONCAT(AQ44,"Q ",AR44,":",TEXT(AS44,"00")),"")</f>
         <v/>
       </c>
@@ -6747,7 +6743,7 @@
         <f aca="false">IF(AT44="","",IF(AT45="",AV44,AT44-AT45))</f>
         <v/>
       </c>
-      <c r="BF44" s="8" t="n">
+      <c r="BF44" s="7" t="n">
         <f aca="false">BE44=AV44</f>
         <v>1</v>
       </c>
@@ -6772,7 +6768,7 @@
         <f aca="false">IF(E45="","",IF(E44="",1,1+J44))</f>
         <v/>
       </c>
-      <c r="N45" s="7" t="str">
+      <c r="N45" s="2" t="str">
         <f aca="false">IF(G45="?",_xlfn.CONCAT(AQ45,"Q ",AR45,":",TEXT(AS45,"00")),"")</f>
         <v/>
       </c>
@@ -6792,7 +6788,7 @@
         <f aca="false">IF(AT45="","",IF(AT46="",AV45,AT45-AT46))</f>
         <v/>
       </c>
-      <c r="BF45" s="8" t="n">
+      <c r="BF45" s="7" t="n">
         <f aca="false">BE45=AV45</f>
         <v>1</v>
       </c>
@@ -6817,7 +6813,7 @@
         <f aca="false">IF(E46="","",IF(E45="",1,1+J45))</f>
         <v/>
       </c>
-      <c r="N46" s="7" t="str">
+      <c r="N46" s="2" t="str">
         <f aca="false">IF(G46="?",_xlfn.CONCAT(AQ46,"Q ",AR46,":",TEXT(AS46,"00")),"")</f>
         <v/>
       </c>
@@ -6837,7 +6833,7 @@
         <f aca="false">IF(AT46="","",IF(AT47="",AV46,AT46-AT47))</f>
         <v/>
       </c>
-      <c r="BF46" s="8" t="n">
+      <c r="BF46" s="7" t="n">
         <f aca="false">BE46=AV46</f>
         <v>1</v>
       </c>
@@ -6862,7 +6858,7 @@
         <f aca="false">IF(E47="","",IF(E46="",1,1+J46))</f>
         <v/>
       </c>
-      <c r="N47" s="7" t="str">
+      <c r="N47" s="2" t="str">
         <f aca="false">IF(G47="?",_xlfn.CONCAT(AQ47,"Q ",AR47,":",TEXT(AS47,"00")),"")</f>
         <v/>
       </c>
@@ -6882,7 +6878,7 @@
         <f aca="false">IF(AT47="","",IF(AT48="",AV47,AT47-AT48))</f>
         <v/>
       </c>
-      <c r="BF47" s="8" t="n">
+      <c r="BF47" s="7" t="n">
         <f aca="false">BE47=AV47</f>
         <v>1</v>
       </c>
@@ -6907,7 +6903,7 @@
         <f aca="false">IF(E48="","",IF(E47="",1,1+J47))</f>
         <v/>
       </c>
-      <c r="N48" s="7" t="str">
+      <c r="N48" s="2" t="str">
         <f aca="false">IF(G48="?",_xlfn.CONCAT(AQ48,"Q ",AR48,":",TEXT(AS48,"00")),"")</f>
         <v/>
       </c>
@@ -6927,7 +6923,7 @@
         <f aca="false">IF(AT48="","",IF(AT49="",AV48,AT48-AT49))</f>
         <v/>
       </c>
-      <c r="BF48" s="8" t="n">
+      <c r="BF48" s="7" t="n">
         <f aca="false">BE48=AV48</f>
         <v>1</v>
       </c>
@@ -6952,7 +6948,7 @@
         <f aca="false">IF(E49="","",IF(E48="",1,1+J48))</f>
         <v/>
       </c>
-      <c r="N49" s="7" t="str">
+      <c r="N49" s="2" t="str">
         <f aca="false">IF(G49="?",_xlfn.CONCAT(AQ49,"Q ",AR49,":",TEXT(AS49,"00")),"")</f>
         <v/>
       </c>
@@ -6972,7 +6968,7 @@
         <f aca="false">IF(AT49="","",IF(AT50="",AV49,AT49-AT50))</f>
         <v/>
       </c>
-      <c r="BF49" s="8" t="n">
+      <c r="BF49" s="7" t="n">
         <f aca="false">BE49=AV49</f>
         <v>1</v>
       </c>
@@ -6997,7 +6993,7 @@
         <f aca="false">IF(E50="","",IF(E49="",1,1+J49))</f>
         <v/>
       </c>
-      <c r="N50" s="7" t="str">
+      <c r="N50" s="2" t="str">
         <f aca="false">IF(G50="?",_xlfn.CONCAT(AQ50,"Q ",AR50,":",TEXT(AS50,"00")),"")</f>
         <v/>
       </c>
@@ -7017,7 +7013,7 @@
         <f aca="false">IF(AT50="","",IF(AT51="",AV50,AT50-AT51))</f>
         <v/>
       </c>
-      <c r="BF50" s="8" t="n">
+      <c r="BF50" s="7" t="n">
         <f aca="false">BE50=AV50</f>
         <v>1</v>
       </c>
@@ -7042,7 +7038,7 @@
         <f aca="false">IF(E51="","",IF(E50="",1,1+J50))</f>
         <v/>
       </c>
-      <c r="N51" s="7" t="str">
+      <c r="N51" s="2" t="str">
         <f aca="false">IF(G51="?",_xlfn.CONCAT(AQ51,"Q ",AR51,":",TEXT(AS51,"00")),"")</f>
         <v/>
       </c>
@@ -7062,7 +7058,7 @@
         <f aca="false">IF(AT51="","",IF(AT52="",AV51,AT51-AT52))</f>
         <v/>
       </c>
-      <c r="BF51" s="8" t="n">
+      <c r="BF51" s="7" t="n">
         <f aca="false">BE51=AV51</f>
         <v>1</v>
       </c>
@@ -7087,7 +7083,7 @@
         <f aca="false">IF(E52="","",IF(E51="",1,1+J51))</f>
         <v/>
       </c>
-      <c r="N52" s="7" t="str">
+      <c r="N52" s="2" t="str">
         <f aca="false">IF(G52="?",_xlfn.CONCAT(AQ52,"Q ",AR52,":",TEXT(AS52,"00")),"")</f>
         <v/>
       </c>
@@ -7107,7 +7103,7 @@
         <f aca="false">IF(AT52="","",IF(AT53="",AV52,AT52-AT53))</f>
         <v/>
       </c>
-      <c r="BF52" s="8" t="n">
+      <c r="BF52" s="7" t="n">
         <f aca="false">BE52=AV52</f>
         <v>1</v>
       </c>
@@ -7132,7 +7128,7 @@
         <f aca="false">IF(E53="","",IF(E52="",1,1+J52))</f>
         <v/>
       </c>
-      <c r="N53" s="7" t="str">
+      <c r="N53" s="2" t="str">
         <f aca="false">IF(G53="?",_xlfn.CONCAT(AQ53,"Q ",AR53,":",TEXT(AS53,"00")),"")</f>
         <v/>
       </c>
@@ -7152,7 +7148,7 @@
         <f aca="false">IF(AT53="","",IF(AT54="",AV53,AT53-AT54))</f>
         <v/>
       </c>
-      <c r="BF53" s="8" t="n">
+      <c r="BF53" s="7" t="n">
         <f aca="false">BE53=AV53</f>
         <v>1</v>
       </c>
@@ -7177,7 +7173,7 @@
         <f aca="false">IF(E54="","",IF(E53="",1,1+J53))</f>
         <v/>
       </c>
-      <c r="N54" s="7" t="str">
+      <c r="N54" s="2" t="str">
         <f aca="false">IF(G54="?",_xlfn.CONCAT(AQ54,"Q ",AR54,":",TEXT(AS54,"00")),"")</f>
         <v/>
       </c>
@@ -7197,7 +7193,7 @@
         <f aca="false">IF(AT54="","",IF(AT55="",AV54,AT54-AT55))</f>
         <v/>
       </c>
-      <c r="BF54" s="8" t="n">
+      <c r="BF54" s="7" t="n">
         <f aca="false">BE54=AV54</f>
         <v>1</v>
       </c>
@@ -7222,7 +7218,7 @@
         <f aca="false">IF(E55="","",IF(E54="",1,1+J54))</f>
         <v/>
       </c>
-      <c r="N55" s="7" t="str">
+      <c r="N55" s="2" t="str">
         <f aca="false">IF(G55="?",_xlfn.CONCAT(AQ55,"Q ",AR55,":",TEXT(AS55,"00")),"")</f>
         <v/>
       </c>
@@ -7242,7 +7238,7 @@
         <f aca="false">IF(AT55="","",IF(AT56="",AV55,AT55-AT56))</f>
         <v/>
       </c>
-      <c r="BF55" s="8" t="n">
+      <c r="BF55" s="7" t="n">
         <f aca="false">BE55=AV55</f>
         <v>1</v>
       </c>
@@ -7267,7 +7263,7 @@
         <f aca="false">IF(E56="","",IF(E55="",1,1+J55))</f>
         <v/>
       </c>
-      <c r="N56" s="7" t="str">
+      <c r="N56" s="2" t="str">
         <f aca="false">IF(G56="?",_xlfn.CONCAT(AQ56,"Q ",AR56,":",TEXT(AS56,"00")),"")</f>
         <v/>
       </c>
@@ -7287,7 +7283,7 @@
         <f aca="false">IF(AT56="","",IF(AT57="",AV56,AT56-AT57))</f>
         <v/>
       </c>
-      <c r="BF56" s="8" t="n">
+      <c r="BF56" s="7" t="n">
         <f aca="false">BE56=AV56</f>
         <v>1</v>
       </c>
@@ -7312,7 +7308,7 @@
         <f aca="false">IF(E57="","",IF(E56="",1,1+J56))</f>
         <v/>
       </c>
-      <c r="N57" s="7" t="str">
+      <c r="N57" s="2" t="str">
         <f aca="false">IF(G57="?",_xlfn.CONCAT(AQ57,"Q ",AR57,":",TEXT(AS57,"00")),"")</f>
         <v/>
       </c>
@@ -7332,7 +7328,7 @@
         <f aca="false">IF(AT57="","",IF(AT58="",AV57,AT57-AT58))</f>
         <v/>
       </c>
-      <c r="BF57" s="8" t="n">
+      <c r="BF57" s="7" t="n">
         <f aca="false">BE57=AV57</f>
         <v>1</v>
       </c>
@@ -7357,7 +7353,7 @@
         <f aca="false">IF(E58="","",IF(E57="",1,1+J57))</f>
         <v/>
       </c>
-      <c r="N58" s="7" t="str">
+      <c r="N58" s="2" t="str">
         <f aca="false">IF(G58="?",_xlfn.CONCAT(AQ58,"Q ",AR58,":",TEXT(AS58,"00")),"")</f>
         <v/>
       </c>
@@ -7377,7 +7373,7 @@
         <f aca="false">IF(AT58="","",IF(AT59="",AV58,AT58-AT59))</f>
         <v/>
       </c>
-      <c r="BF58" s="8" t="n">
+      <c r="BF58" s="7" t="n">
         <f aca="false">BE58=AV58</f>
         <v>1</v>
       </c>
@@ -7402,7 +7398,7 @@
         <f aca="false">IF(E59="","",IF(E58="",1,1+J58))</f>
         <v/>
       </c>
-      <c r="N59" s="7" t="str">
+      <c r="N59" s="2" t="str">
         <f aca="false">IF(G59="?",_xlfn.CONCAT(AQ59,"Q ",AR59,":",TEXT(AS59,"00")),"")</f>
         <v/>
       </c>
@@ -7422,7 +7418,7 @@
         <f aca="false">IF(AT59="","",IF(AT60="",AV59,AT59-AT60))</f>
         <v/>
       </c>
-      <c r="BF59" s="8" t="n">
+      <c r="BF59" s="7" t="n">
         <f aca="false">BE59=AV59</f>
         <v>1</v>
       </c>
@@ -7447,7 +7443,7 @@
         <f aca="false">IF(E60="","",IF(E59="",1,1+J59))</f>
         <v/>
       </c>
-      <c r="N60" s="7" t="str">
+      <c r="N60" s="2" t="str">
         <f aca="false">IF(G60="?",_xlfn.CONCAT(AQ60,"Q ",AR60,":",TEXT(AS60,"00")),"")</f>
         <v/>
       </c>
@@ -7467,7 +7463,7 @@
         <f aca="false">IF(AT60="","",IF(AT61="",AV60,AT60-AT61))</f>
         <v/>
       </c>
-      <c r="BF60" s="8" t="n">
+      <c r="BF60" s="7" t="n">
         <f aca="false">BE60=AV60</f>
         <v>1</v>
       </c>
@@ -7492,7 +7488,7 @@
         <f aca="false">IF(E61="","",IF(E60="",1,1+J60))</f>
         <v/>
       </c>
-      <c r="N61" s="7" t="str">
+      <c r="N61" s="2" t="str">
         <f aca="false">IF(G61="?",_xlfn.CONCAT(AQ61,"Q ",AR61,":",TEXT(AS61,"00")),"")</f>
         <v/>
       </c>
@@ -7512,7 +7508,7 @@
         <f aca="false">IF(AT61="","",IF(AT62="",AV61,AT61-AT62))</f>
         <v/>
       </c>
-      <c r="BF61" s="8" t="n">
+      <c r="BF61" s="7" t="n">
         <f aca="false">BE61=AV61</f>
         <v>1</v>
       </c>
@@ -7537,7 +7533,7 @@
         <f aca="false">IF(E62="","",IF(E61="",1,1+J61))</f>
         <v/>
       </c>
-      <c r="N62" s="7" t="str">
+      <c r="N62" s="2" t="str">
         <f aca="false">IF(G62="?",_xlfn.CONCAT(AQ62,"Q ",AR62,":",TEXT(AS62,"00")),"")</f>
         <v/>
       </c>
@@ -7557,7 +7553,7 @@
         <f aca="false">IF(AT62="","",IF(AT63="",AV62,AT62-AT63))</f>
         <v/>
       </c>
-      <c r="BF62" s="8" t="n">
+      <c r="BF62" s="7" t="n">
         <f aca="false">BE62=AV62</f>
         <v>1</v>
       </c>
@@ -7582,7 +7578,7 @@
         <f aca="false">IF(E63="","",IF(E62="",1,1+J62))</f>
         <v/>
       </c>
-      <c r="N63" s="7" t="str">
+      <c r="N63" s="2" t="str">
         <f aca="false">IF(G63="?",_xlfn.CONCAT(AQ63,"Q ",AR63,":",TEXT(AS63,"00")),"")</f>
         <v/>
       </c>
@@ -7602,7 +7598,7 @@
         <f aca="false">IF(AT63="","",IF(AT64="",AV63,AT63-AT64))</f>
         <v/>
       </c>
-      <c r="BF63" s="8" t="n">
+      <c r="BF63" s="7" t="n">
         <f aca="false">BE63=AV63</f>
         <v>1</v>
       </c>
@@ -7627,7 +7623,7 @@
         <f aca="false">IF(E64="","",IF(E63="",1,1+J63))</f>
         <v/>
       </c>
-      <c r="N64" s="7" t="str">
+      <c r="N64" s="2" t="str">
         <f aca="false">IF(G64="?",_xlfn.CONCAT(AQ64,"Q ",AR64,":",TEXT(AS64,"00")),"")</f>
         <v/>
       </c>
@@ -7647,7 +7643,7 @@
         <f aca="false">IF(AT64="","",IF(AT65="",AV64,AT64-AT65))</f>
         <v/>
       </c>
-      <c r="BF64" s="8" t="n">
+      <c r="BF64" s="7" t="n">
         <f aca="false">BE64=AV64</f>
         <v>1</v>
       </c>
@@ -7672,7 +7668,7 @@
         <f aca="false">IF(E65="","",IF(E64="",1,1+J64))</f>
         <v/>
       </c>
-      <c r="N65" s="7" t="str">
+      <c r="N65" s="2" t="str">
         <f aca="false">IF(G65="?",_xlfn.CONCAT(AQ65,"Q ",AR65,":",TEXT(AS65,"00")),"")</f>
         <v/>
       </c>
@@ -7692,7 +7688,7 @@
         <f aca="false">IF(AT65="","",IF(AT66="",AV65,AT65-AT66))</f>
         <v/>
       </c>
-      <c r="BF65" s="8" t="n">
+      <c r="BF65" s="7" t="n">
         <f aca="false">BE65=AV65</f>
         <v>1</v>
       </c>
@@ -7717,7 +7713,7 @@
         <f aca="false">IF(E66="","",IF(E65="",1,1+J65))</f>
         <v/>
       </c>
-      <c r="N66" s="7" t="str">
+      <c r="N66" s="2" t="str">
         <f aca="false">IF(G66="?",_xlfn.CONCAT(AQ66,"Q ",AR66,":",TEXT(AS66,"00")),"")</f>
         <v/>
       </c>
@@ -7737,7 +7733,7 @@
         <f aca="false">IF(AT66="","",IF(AT67="",AV66,AT66-AT67))</f>
         <v/>
       </c>
-      <c r="BF66" s="8" t="n">
+      <c r="BF66" s="7" t="n">
         <f aca="false">BE66=AV66</f>
         <v>1</v>
       </c>
@@ -7762,7 +7758,7 @@
         <f aca="false">IF(E67="","",IF(E66="",1,1+J66))</f>
         <v/>
       </c>
-      <c r="N67" s="7" t="str">
+      <c r="N67" s="2" t="str">
         <f aca="false">IF(G67="?",_xlfn.CONCAT(AQ67,"Q ",AR67,":",TEXT(AS67,"00")),"")</f>
         <v/>
       </c>
@@ -7782,7 +7778,7 @@
         <f aca="false">IF(AT67="","",IF(AT68="",AV67,AT67-AT68))</f>
         <v/>
       </c>
-      <c r="BF67" s="8" t="n">
+      <c r="BF67" s="7" t="n">
         <f aca="false">BE67=AV67</f>
         <v>1</v>
       </c>
@@ -7807,7 +7803,7 @@
         <f aca="false">IF(E68="","",IF(E67="",1,1+J67))</f>
         <v/>
       </c>
-      <c r="N68" s="7" t="str">
+      <c r="N68" s="2" t="str">
         <f aca="false">IF(G68="?",_xlfn.CONCAT(AQ68,"Q ",AR68,":",TEXT(AS68,"00")),"")</f>
         <v/>
       </c>
@@ -7827,7 +7823,7 @@
         <f aca="false">IF(AT68="","",IF(AT69="",AV68,AT68-AT69))</f>
         <v/>
       </c>
-      <c r="BF68" s="8" t="n">
+      <c r="BF68" s="7" t="n">
         <f aca="false">BE68=AV68</f>
         <v>1</v>
       </c>
@@ -7852,7 +7848,7 @@
         <f aca="false">IF(E69="","",IF(E68="",1,1+J68))</f>
         <v/>
       </c>
-      <c r="N69" s="7" t="str">
+      <c r="N69" s="2" t="str">
         <f aca="false">IF(G69="?",_xlfn.CONCAT(AQ69,"Q ",AR69,":",TEXT(AS69,"00")),"")</f>
         <v/>
       </c>
@@ -7872,7 +7868,7 @@
         <f aca="false">IF(AT69="","",IF(AT70="",AV69,AT69-AT70))</f>
         <v/>
       </c>
-      <c r="BF69" s="8" t="n">
+      <c r="BF69" s="7" t="n">
         <f aca="false">BE69=AV69</f>
         <v>1</v>
       </c>
@@ -7897,7 +7893,7 @@
         <f aca="false">IF(E70="","",IF(E69="",1,1+J69))</f>
         <v/>
       </c>
-      <c r="N70" s="7" t="str">
+      <c r="N70" s="2" t="str">
         <f aca="false">IF(G70="?",_xlfn.CONCAT(AQ70,"Q ",AR70,":",TEXT(AS70,"00")),"")</f>
         <v/>
       </c>
@@ -7917,7 +7913,7 @@
         <f aca="false">IF(AT70="","",IF(AT71="",AV70,AT70-AT71))</f>
         <v/>
       </c>
-      <c r="BF70" s="8" t="n">
+      <c r="BF70" s="7" t="n">
         <f aca="false">BE70=AV70</f>
         <v>1</v>
       </c>
@@ -7942,7 +7938,7 @@
         <f aca="false">IF(E71="","",IF(E70="",1,1+J70))</f>
         <v/>
       </c>
-      <c r="N71" s="7" t="str">
+      <c r="N71" s="2" t="str">
         <f aca="false">IF(G71="?",_xlfn.CONCAT(AQ71,"Q ",AR71,":",TEXT(AS71,"00")),"")</f>
         <v/>
       </c>
@@ -7962,7 +7958,7 @@
         <f aca="false">IF(AT71="","",IF(AT72="",AV71,AT71-AT72))</f>
         <v/>
       </c>
-      <c r="BF71" s="8" t="n">
+      <c r="BF71" s="7" t="n">
         <f aca="false">BE71=AV71</f>
         <v>1</v>
       </c>
@@ -7987,7 +7983,7 @@
         <f aca="false">IF(E72="","",IF(E71="",1,1+J71))</f>
         <v/>
       </c>
-      <c r="N72" s="7" t="str">
+      <c r="N72" s="2" t="str">
         <f aca="false">IF(G72="?",_xlfn.CONCAT(AQ72,"Q ",AR72,":",TEXT(AS72,"00")),"")</f>
         <v/>
       </c>
@@ -8007,7 +8003,7 @@
         <f aca="false">IF(AT72="","",IF(AT73="",AV72,AT72-AT73))</f>
         <v/>
       </c>
-      <c r="BF72" s="8" t="n">
+      <c r="BF72" s="7" t="n">
         <f aca="false">BE72=AV72</f>
         <v>1</v>
       </c>
@@ -8032,7 +8028,7 @@
         <f aca="false">IF(E73="","",IF(E72="",1,1+J72))</f>
         <v/>
       </c>
-      <c r="N73" s="7" t="str">
+      <c r="N73" s="2" t="str">
         <f aca="false">IF(G73="?",_xlfn.CONCAT(AQ73,"Q ",AR73,":",TEXT(AS73,"00")),"")</f>
         <v/>
       </c>
@@ -8052,7 +8048,7 @@
         <f aca="false">IF(AT73="","",IF(AT74="",AV73,AT73-AT74))</f>
         <v/>
       </c>
-      <c r="BF73" s="8" t="n">
+      <c r="BF73" s="7" t="n">
         <f aca="false">BE73=AV73</f>
         <v>1</v>
       </c>
@@ -8077,7 +8073,7 @@
         <f aca="false">IF(E74="","",IF(E73="",1,1+J73))</f>
         <v/>
       </c>
-      <c r="N74" s="7" t="str">
+      <c r="N74" s="2" t="str">
         <f aca="false">IF(G74="?",_xlfn.CONCAT(AQ74,"Q ",AR74,":",TEXT(AS74,"00")),"")</f>
         <v/>
       </c>
@@ -8097,7 +8093,7 @@
         <f aca="false">IF(AT74="","",IF(AT75="",AV74,AT74-AT75))</f>
         <v/>
       </c>
-      <c r="BF74" s="8" t="n">
+      <c r="BF74" s="7" t="n">
         <f aca="false">BE74=AV74</f>
         <v>1</v>
       </c>
@@ -8122,7 +8118,7 @@
         <f aca="false">IF(E75="","",IF(E74="",1,1+J74))</f>
         <v/>
       </c>
-      <c r="N75" s="7" t="str">
+      <c r="N75" s="2" t="str">
         <f aca="false">IF(G75="?",_xlfn.CONCAT(AQ75,"Q ",AR75,":",TEXT(AS75,"00")),"")</f>
         <v/>
       </c>
@@ -8142,7 +8138,7 @@
         <f aca="false">IF(AT75="","",IF(AT76="",AV75,AT75-AT76))</f>
         <v/>
       </c>
-      <c r="BF75" s="8" t="n">
+      <c r="BF75" s="7" t="n">
         <f aca="false">BE75=AV75</f>
         <v>1</v>
       </c>
@@ -8167,7 +8163,7 @@
         <f aca="false">IF(E76="","",IF(E75="",1,1+J75))</f>
         <v/>
       </c>
-      <c r="N76" s="7" t="str">
+      <c r="N76" s="2" t="str">
         <f aca="false">IF(G76="?",_xlfn.CONCAT(AQ76,"Q ",AR76,":",TEXT(AS76,"00")),"")</f>
         <v/>
       </c>
@@ -8187,7 +8183,7 @@
         <f aca="false">IF(AT76="","",IF(AT77="",AV76,AT76-AT77))</f>
         <v/>
       </c>
-      <c r="BF76" s="8" t="n">
+      <c r="BF76" s="7" t="n">
         <f aca="false">BE76=AV76</f>
         <v>1</v>
       </c>
@@ -8212,7 +8208,6 @@
         <f aca="false">IF(E77="","",IF(E76="",1,1+J76))</f>
         <v/>
       </c>
-      <c r="N77" s="7"/>
       <c r="AI77" s="2"/>
       <c r="AJ77" s="1" t="str">
         <f aca="false">IF(K77="t","o",IF(E78="1st","o","d"))</f>
@@ -8231,7 +8226,7 @@
         <f aca="false">IF(AT77="","",IF(AT78="",AV77,AT77-AT78))</f>
         <v/>
       </c>
-      <c r="BF77" s="8" t="n">
+      <c r="BF77" s="7" t="n">
         <f aca="false">BE77=AV77</f>
         <v>1</v>
       </c>
@@ -8256,7 +8251,6 @@
         <f aca="false">IF(E78="","",IF(E77="",1,1+J77))</f>
         <v/>
       </c>
-      <c r="N78" s="7"/>
       <c r="AI78" s="2"/>
       <c r="AJ78" s="1" t="str">
         <f aca="false">IF(K78="t","o",IF(E79="1st","o","d"))</f>
@@ -8275,7 +8269,7 @@
         <f aca="false">IF(AT78="","",IF(AT79="",AV78,AT78-AT79))</f>
         <v/>
       </c>
-      <c r="BF78" s="8" t="n">
+      <c r="BF78" s="7" t="n">
         <f aca="false">BE78=AV78</f>
         <v>1</v>
       </c>
@@ -8300,7 +8294,6 @@
         <f aca="false">IF(E79="","",IF(E78="",1,1+J78))</f>
         <v/>
       </c>
-      <c r="N79" s="7"/>
       <c r="AI79" s="2"/>
       <c r="AJ79" s="1" t="str">
         <f aca="false">IF(K79="t","o",IF(E80="1st","o","d"))</f>
@@ -8319,7 +8312,7 @@
         <f aca="false">IF(AT79="","",IF(AT80="",AV79,AT79-AT80))</f>
         <v/>
       </c>
-      <c r="BF79" s="8" t="n">
+      <c r="BF79" s="7" t="n">
         <f aca="false">BE79=AV79</f>
         <v>1</v>
       </c>
@@ -8344,7 +8337,6 @@
         <f aca="false">IF(E80="","",IF(E79="",1,1+J79))</f>
         <v/>
       </c>
-      <c r="N80" s="7"/>
       <c r="AI80" s="2"/>
       <c r="AJ80" s="1" t="str">
         <f aca="false">IF(K80="t","o",IF(E81="1st","o","d"))</f>
@@ -8363,7 +8355,7 @@
         <f aca="false">IF(AT80="","",IF(AT81="",AV80,AT80-AT81))</f>
         <v/>
       </c>
-      <c r="BF80" s="8" t="n">
+      <c r="BF80" s="7" t="n">
         <f aca="false">BE80=AV80</f>
         <v>1</v>
       </c>
@@ -8388,7 +8380,6 @@
         <f aca="false">IF(E81="","",IF(E80="",1,1+J80))</f>
         <v/>
       </c>
-      <c r="N81" s="7"/>
       <c r="AI81" s="2"/>
       <c r="AJ81" s="1" t="str">
         <f aca="false">IF(K81="t","o",IF(E82="1st","o","d"))</f>
@@ -8407,7 +8398,7 @@
         <f aca="false">IF(AT81="","",IF(AT82="",AV81,AT81-AT82))</f>
         <v/>
       </c>
-      <c r="BF81" s="8" t="n">
+      <c r="BF81" s="7" t="n">
         <f aca="false">BE81=AV81</f>
         <v>1</v>
       </c>
@@ -8432,7 +8423,6 @@
         <f aca="false">IF(E82="","",IF(E81="",1,1+J81))</f>
         <v/>
       </c>
-      <c r="N82" s="7"/>
       <c r="AI82" s="2"/>
       <c r="AJ82" s="1" t="str">
         <f aca="false">IF(K82="t","o",IF(E83="1st","o","d"))</f>
@@ -8451,7 +8441,7 @@
         <f aca="false">IF(AT82="","",IF(AT83="",AV82,AT82-AT83))</f>
         <v/>
       </c>
-      <c r="BF82" s="8" t="n">
+      <c r="BF82" s="7" t="n">
         <f aca="false">BE82=AV82</f>
         <v>1</v>
       </c>
@@ -8476,7 +8466,6 @@
         <f aca="false">IF(E83="","",IF(E82="",1,1+J82))</f>
         <v/>
       </c>
-      <c r="N83" s="7"/>
       <c r="AI83" s="2"/>
       <c r="AJ83" s="1" t="str">
         <f aca="false">IF(K83="t","o",IF(E84="1st","o","d"))</f>
@@ -8495,7 +8484,7 @@
         <f aca="false">IF(AT83="","",IF(AT84="",AV83,AT83-AT84))</f>
         <v/>
       </c>
-      <c r="BF83" s="8" t="n">
+      <c r="BF83" s="7" t="n">
         <f aca="false">BE83=AV83</f>
         <v>1</v>
       </c>
@@ -8520,7 +8509,6 @@
         <f aca="false">IF(E84="","",IF(E83="",1,1+J83))</f>
         <v/>
       </c>
-      <c r="N84" s="7"/>
       <c r="AI84" s="2"/>
       <c r="AJ84" s="1" t="str">
         <f aca="false">IF(K84="t","o",IF(E85="1st","o","d"))</f>
@@ -8539,7 +8527,7 @@
         <f aca="false">IF(AT84="","",IF(AT85="",AV84,AT84-AT85))</f>
         <v/>
       </c>
-      <c r="BF84" s="8" t="n">
+      <c r="BF84" s="7" t="n">
         <f aca="false">BE84=AV84</f>
         <v>1</v>
       </c>
@@ -8564,7 +8552,6 @@
         <f aca="false">IF(E85="","",IF(E84="",1,1+J84))</f>
         <v/>
       </c>
-      <c r="N85" s="7"/>
       <c r="AI85" s="2"/>
       <c r="AJ85" s="1" t="str">
         <f aca="false">IF(K85="t","o",IF(E86="1st","o","d"))</f>
@@ -8583,7 +8570,7 @@
         <f aca="false">IF(AT85="","",IF(AT86="",AV85,AT85-AT86))</f>
         <v/>
       </c>
-      <c r="BF85" s="8" t="n">
+      <c r="BF85" s="7" t="n">
         <f aca="false">BE85=AV85</f>
         <v>1</v>
       </c>
@@ -8608,7 +8595,6 @@
         <f aca="false">IF(E86="","",IF(E85="",1,1+J85))</f>
         <v/>
       </c>
-      <c r="N86" s="7"/>
       <c r="AI86" s="2"/>
       <c r="AJ86" s="1" t="str">
         <f aca="false">IF(K86="t","o",IF(E87="1st","o","d"))</f>
@@ -8627,7 +8613,7 @@
         <f aca="false">IF(AT86="","",IF(AT87="",AV86,AT86-AT87))</f>
         <v/>
       </c>
-      <c r="BF86" s="8" t="n">
+      <c r="BF86" s="7" t="n">
         <f aca="false">BE86=AV86</f>
         <v>1</v>
       </c>
@@ -8652,7 +8638,6 @@
         <f aca="false">IF(E87="","",IF(E86="",1,1+J86))</f>
         <v/>
       </c>
-      <c r="N87" s="7"/>
       <c r="AI87" s="2"/>
       <c r="AJ87" s="1" t="str">
         <f aca="false">IF(K87="t","o",IF(E88="1st","o","d"))</f>
@@ -8671,7 +8656,7 @@
         <f aca="false">IF(AT87="","",IF(AT88="",AV87,AT87-AT88))</f>
         <v/>
       </c>
-      <c r="BF87" s="8" t="n">
+      <c r="BF87" s="7" t="n">
         <f aca="false">BE87=AV87</f>
         <v>1</v>
       </c>
@@ -8696,7 +8681,6 @@
         <f aca="false">IF(E88="","",IF(E87="",1,1+J87))</f>
         <v/>
       </c>
-      <c r="N88" s="7"/>
       <c r="AI88" s="2"/>
       <c r="AJ88" s="1" t="str">
         <f aca="false">IF(K88="t","o",IF(E89="1st","o","d"))</f>
@@ -8714,7 +8698,7 @@
         <f aca="false">IF(AT88="","",IF(AT89="",AV88,AT88-AT89))</f>
         <v/>
       </c>
-      <c r="BF88" s="8" t="n">
+      <c r="BF88" s="7" t="n">
         <f aca="false">BE88=AV88</f>
         <v>1</v>
       </c>
@@ -8739,7 +8723,6 @@
         <f aca="false">IF(E89="","",IF(E88="",1,1+J88))</f>
         <v/>
       </c>
-      <c r="N89" s="7"/>
       <c r="AI89" s="2"/>
       <c r="AJ89" s="1" t="str">
         <f aca="false">IF(K89="t","o",IF(E90="1st","o","d"))</f>
@@ -8758,7 +8741,7 @@
         <f aca="false">IF(AT89="","",IF(AT90="",AV89,AT89-AT90))</f>
         <v/>
       </c>
-      <c r="BF89" s="8" t="n">
+      <c r="BF89" s="7" t="n">
         <f aca="false">BE89=AV89</f>
         <v>1</v>
       </c>
@@ -8783,7 +8766,6 @@
         <f aca="false">IF(E90="","",IF(E89="",1,1+J89))</f>
         <v/>
       </c>
-      <c r="N90" s="7"/>
       <c r="AI90" s="2"/>
       <c r="AJ90" s="1" t="str">
         <f aca="false">IF(K90="t","o",IF(E91="1st","o","d"))</f>
@@ -8802,7 +8784,7 @@
         <f aca="false">IF(AT90="","",IF(AT91="",AV90,AT90-AT91))</f>
         <v/>
       </c>
-      <c r="BF90" s="8" t="n">
+      <c r="BF90" s="7" t="n">
         <f aca="false">BE90=AV90</f>
         <v>1</v>
       </c>
@@ -8827,7 +8809,6 @@
         <f aca="false">IF(E91="","",IF(E90="",1,1+J90))</f>
         <v/>
       </c>
-      <c r="N91" s="7"/>
       <c r="AI91" s="2"/>
       <c r="AJ91" s="1" t="str">
         <f aca="false">IF(K91="t","o",IF(E92="1st","o","d"))</f>
@@ -8846,7 +8827,7 @@
         <f aca="false">IF(AT91="","",IF(AT92="",AV91,AT91-AT92))</f>
         <v/>
       </c>
-      <c r="BF91" s="8" t="n">
+      <c r="BF91" s="7" t="n">
         <f aca="false">BE91=AV91</f>
         <v>1</v>
       </c>
@@ -8871,7 +8852,6 @@
         <f aca="false">IF(E92="","",IF(E91="",1,1+J91))</f>
         <v/>
       </c>
-      <c r="N92" s="7"/>
       <c r="AI92" s="2"/>
       <c r="AJ92" s="1" t="str">
         <f aca="false">IF(K92="t","o",IF(E93="1st","o","d"))</f>
@@ -8890,7 +8870,7 @@
         <f aca="false">IF(AT92="","",IF(AT93="",AV92,AT92-AT93))</f>
         <v/>
       </c>
-      <c r="BF92" s="8" t="n">
+      <c r="BF92" s="7" t="n">
         <f aca="false">BE92=AV92</f>
         <v>1</v>
       </c>
@@ -8915,7 +8895,6 @@
         <f aca="false">IF(E93="","",IF(E92="",1,1+J92))</f>
         <v/>
       </c>
-      <c r="N93" s="7"/>
       <c r="AI93" s="2"/>
       <c r="AJ93" s="1" t="str">
         <f aca="false">IF(K93="t","o",IF(E94="1st","o","d"))</f>
@@ -8934,7 +8913,7 @@
         <f aca="false">IF(AT93="","",IF(AT94="",AV93,AT93-AT94))</f>
         <v/>
       </c>
-      <c r="BF93" s="8" t="n">
+      <c r="BF93" s="7" t="n">
         <f aca="false">BE93=AV93</f>
         <v>1</v>
       </c>
@@ -8959,7 +8938,6 @@
         <f aca="false">IF(E94="","",IF(E93="",1,1+J93))</f>
         <v/>
       </c>
-      <c r="N94" s="7"/>
       <c r="AI94" s="2"/>
       <c r="AJ94" s="1" t="str">
         <f aca="false">IF(K94="t","o",IF(E95="1st","o","d"))</f>
@@ -8978,7 +8956,7 @@
         <f aca="false">IF(AT94="","",IF(AT95="",AV94,AT94-AT95))</f>
         <v/>
       </c>
-      <c r="BF94" s="8" t="n">
+      <c r="BF94" s="7" t="n">
         <f aca="false">BE94=AV94</f>
         <v>1</v>
       </c>
@@ -9003,7 +8981,6 @@
         <f aca="false">IF(E95="","",IF(E94="",1,1+J94))</f>
         <v/>
       </c>
-      <c r="N95" s="7"/>
       <c r="AI95" s="2"/>
       <c r="AJ95" s="1" t="str">
         <f aca="false">IF(K95="t","o",IF(E96="1st","o","d"))</f>
@@ -9022,7 +8999,7 @@
         <f aca="false">IF(AT95="","",IF(AT96="",AV95,AT95-AT96))</f>
         <v/>
       </c>
-      <c r="BF95" s="8" t="n">
+      <c r="BF95" s="7" t="n">
         <f aca="false">BE95=AV95</f>
         <v>1</v>
       </c>
@@ -9047,7 +9024,6 @@
         <f aca="false">IF(E96="","",IF(E95="",1,1+J95))</f>
         <v/>
       </c>
-      <c r="N96" s="7"/>
       <c r="AI96" s="2"/>
       <c r="AJ96" s="1" t="str">
         <f aca="false">IF(K96="t","o",IF(E97="1st","o","d"))</f>
@@ -9066,7 +9042,7 @@
         <f aca="false">IF(AT96="","",IF(AT97="",AV96,AT96-AT97))</f>
         <v/>
       </c>
-      <c r="BF96" s="8" t="n">
+      <c r="BF96" s="7" t="n">
         <f aca="false">BE96=AV96</f>
         <v>1</v>
       </c>
@@ -9091,7 +9067,6 @@
         <f aca="false">IF(E97="","",IF(E96="",1,1+J96))</f>
         <v/>
       </c>
-      <c r="N97" s="7"/>
       <c r="AI97" s="2"/>
       <c r="AJ97" s="1" t="str">
         <f aca="false">IF(K97="t","o",IF(E98="1st","o","d"))</f>
@@ -9110,7 +9085,7 @@
         <f aca="false">IF(AT97="","",IF(AT98="",AV97,AT97-AT98))</f>
         <v/>
       </c>
-      <c r="BF97" s="8" t="n">
+      <c r="BF97" s="7" t="n">
         <f aca="false">BE97=AV97</f>
         <v>1</v>
       </c>
@@ -9135,7 +9110,6 @@
         <f aca="false">IF(E98="","",IF(E97="",1,1+J97))</f>
         <v/>
       </c>
-      <c r="N98" s="7"/>
       <c r="AI98" s="2"/>
       <c r="AJ98" s="1" t="str">
         <f aca="false">IF(K98="t","o",IF(E99="1st","o","d"))</f>
@@ -9154,7 +9128,7 @@
         <f aca="false">IF(AT98="","",IF(AT99="",AV98,AT98-AT99))</f>
         <v/>
       </c>
-      <c r="BF98" s="8" t="n">
+      <c r="BF98" s="7" t="n">
         <f aca="false">BE98=AV98</f>
         <v>1</v>
       </c>
@@ -9179,7 +9153,6 @@
         <f aca="false">IF(E99="","",IF(E98="",1,1+J98))</f>
         <v/>
       </c>
-      <c r="N99" s="7"/>
       <c r="AI99" s="2"/>
       <c r="AJ99" s="1" t="str">
         <f aca="false">IF(K99="t","o",IF(E100="1st","o","d"))</f>
@@ -9198,7 +9171,7 @@
         <f aca="false">IF(AT99="","",IF(AT100="",AV99,AT99-AT100))</f>
         <v/>
       </c>
-      <c r="BF99" s="8" t="n">
+      <c r="BF99" s="7" t="n">
         <f aca="false">BE99=AV99</f>
         <v>1</v>
       </c>
@@ -9223,7 +9196,6 @@
         <f aca="false">IF(E100="","",IF(E99="",1,1+J99))</f>
         <v/>
       </c>
-      <c r="N100" s="7"/>
       <c r="AI100" s="2"/>
       <c r="AJ100" s="1" t="str">
         <f aca="false">IF(K100="t","o",IF(E101="1st","o","d"))</f>
@@ -9242,7 +9214,7 @@
         <f aca="false">IF(AT100="","",IF(AT101="",AV100,AT100-AT101))</f>
         <v/>
       </c>
-      <c r="BF100" s="8" t="n">
+      <c r="BF100" s="7" t="n">
         <f aca="false">BE100=AV100</f>
         <v>1</v>
       </c>

</xml_diff>